<commit_message>
updated presentation and results for base case
</commit_message>
<xml_diff>
--- a/results1.xlsx
+++ b/results1.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18625"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18201"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\William\Workspace\mrFinishLine\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dunnm\Documents\The University of Texas\2017 Fall\CE 391F\Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1005" yWindow="0" windowWidth="27795" windowHeight="12795"/>
+    <workbookView xWindow="1010" yWindow="0" windowWidth="27800" windowHeight="12800"/>
   </bookViews>
   <sheets>
     <sheet name="results1" sheetId="1" r:id="rId1"/>
@@ -18,41 +18,168 @@
     <definedName name="_xlchart.v1.0" hidden="1">results1!$A$10:$LS$10</definedName>
     <definedName name="_xlchart.v1.1" hidden="1">results1!$A$11:$LS$11</definedName>
     <definedName name="_xlchart.v1.10" hidden="1">results1!$A$1:$LS$1</definedName>
-    <definedName name="_xlchart.v1.100" hidden="1">results1!$A$1:$LS$1</definedName>
-    <definedName name="_xlchart.v1.101" hidden="1">results1!$A$20:$LS$20</definedName>
-    <definedName name="_xlchart.v1.102" hidden="1">results1!$A$21:$LS$21</definedName>
-    <definedName name="_xlchart.v1.103" hidden="1">results1!$A$22:$LS$22</definedName>
-    <definedName name="_xlchart.v1.104" hidden="1">results1!$A$23:$LS$23</definedName>
-    <definedName name="_xlchart.v1.105" hidden="1">results1!$A$24:$LS$24</definedName>
-    <definedName name="_xlchart.v1.106" hidden="1">results1!$A$25:$LS$25</definedName>
-    <definedName name="_xlchart.v1.107" hidden="1">results1!$A$26:$LS$26</definedName>
-    <definedName name="_xlchart.v1.108" hidden="1">results1!$A$27:$LS$27</definedName>
-    <definedName name="_xlchart.v1.109" hidden="1">results1!$A$28:$LS$28</definedName>
+    <definedName name="_xlchart.v1.100" hidden="1">results1!$A$18:$LS$18</definedName>
+    <definedName name="_xlchart.v1.101" hidden="1">results1!$A$19:$LS$19</definedName>
+    <definedName name="_xlchart.v1.102" hidden="1">results1!$A$1:$LS$1</definedName>
+    <definedName name="_xlchart.v1.103" hidden="1">results1!$A$20:$LS$20</definedName>
+    <definedName name="_xlchart.v1.104" hidden="1">results1!$A$21:$LS$21</definedName>
+    <definedName name="_xlchart.v1.105" hidden="1">results1!$A$22:$LS$22</definedName>
+    <definedName name="_xlchart.v1.106" hidden="1">results1!$A$23:$LS$23</definedName>
+    <definedName name="_xlchart.v1.107" hidden="1">results1!$A$24:$LS$24</definedName>
+    <definedName name="_xlchart.v1.108" hidden="1">results1!$A$25:$LS$25</definedName>
+    <definedName name="_xlchart.v1.109" hidden="1">results1!$A$26:$LS$26</definedName>
     <definedName name="_xlchart.v1.11" hidden="1">results1!$A$20:$LS$20</definedName>
-    <definedName name="_xlchart.v1.110" hidden="1">results1!$A$29:$LS$29</definedName>
-    <definedName name="_xlchart.v1.111" hidden="1">results1!$A$2:$LS$2</definedName>
-    <definedName name="_xlchart.v1.112" hidden="1">results1!$A$30:$LS$30</definedName>
-    <definedName name="_xlchart.v1.113" hidden="1">results1!$A$3:$LS$3</definedName>
-    <definedName name="_xlchart.v1.114" hidden="1">results1!$A$4:$LS$4</definedName>
-    <definedName name="_xlchart.v1.115" hidden="1">results1!$A$5:$LS$5</definedName>
-    <definedName name="_xlchart.v1.116" hidden="1">results1!$A$6:$LS$6</definedName>
-    <definedName name="_xlchart.v1.117" hidden="1">results1!$A$7:$LS$7</definedName>
-    <definedName name="_xlchart.v1.118" hidden="1">results1!$A$8:$LS$8</definedName>
-    <definedName name="_xlchart.v1.119" hidden="1">results1!$A$9:$LS$9</definedName>
+    <definedName name="_xlchart.v1.110" hidden="1">results1!$A$27:$LS$27</definedName>
+    <definedName name="_xlchart.v1.111" hidden="1">results1!$A$28:$LS$28</definedName>
+    <definedName name="_xlchart.v1.112" hidden="1">results1!$A$29:$LS$29</definedName>
+    <definedName name="_xlchart.v1.113" hidden="1">results1!$A$2:$LS$2</definedName>
+    <definedName name="_xlchart.v1.114" hidden="1">results1!$A$30:$LS$30</definedName>
+    <definedName name="_xlchart.v1.115" hidden="1">results1!$A$3:$LS$3</definedName>
+    <definedName name="_xlchart.v1.116" hidden="1">results1!$A$4:$LS$4</definedName>
+    <definedName name="_xlchart.v1.117" hidden="1">results1!$A$5:$LS$5</definedName>
+    <definedName name="_xlchart.v1.118" hidden="1">results1!$A$6:$LS$6</definedName>
+    <definedName name="_xlchart.v1.119" hidden="1">results1!$A$7:$LS$7</definedName>
     <definedName name="_xlchart.v1.12" hidden="1">results1!$A$21:$LS$21</definedName>
+    <definedName name="_xlchart.v1.120" hidden="1">results1!$A$8:$LS$8</definedName>
+    <definedName name="_xlchart.v1.121" hidden="1">results1!$A$9:$LS$9</definedName>
+    <definedName name="_xlchart.v1.122" hidden="1">results1!$A$9:$LS$9</definedName>
+    <definedName name="_xlchart.v1.123" hidden="1">results1!$A$10:$LS$10</definedName>
+    <definedName name="_xlchart.v1.124" hidden="1">results1!$A$11:$LS$11</definedName>
+    <definedName name="_xlchart.v1.125" hidden="1">results1!$A$12:$LS$12</definedName>
+    <definedName name="_xlchart.v1.126" hidden="1">results1!$A$13:$LS$13</definedName>
+    <definedName name="_xlchart.v1.127" hidden="1">results1!$A$14:$LS$14</definedName>
+    <definedName name="_xlchart.v1.128" hidden="1">results1!$A$15:$LS$15</definedName>
+    <definedName name="_xlchart.v1.129" hidden="1">results1!$A$16:$LS$16</definedName>
     <definedName name="_xlchart.v1.13" hidden="1">results1!$A$22:$LS$22</definedName>
+    <definedName name="_xlchart.v1.130" hidden="1">results1!$A$17:$LS$17</definedName>
+    <definedName name="_xlchart.v1.131" hidden="1">results1!$A$18:$LS$18</definedName>
+    <definedName name="_xlchart.v1.132" hidden="1">results1!$A$19:$LS$19</definedName>
+    <definedName name="_xlchart.v1.133" hidden="1">results1!$A$1:$LS$1</definedName>
+    <definedName name="_xlchart.v1.134" hidden="1">results1!$A$20:$LS$20</definedName>
+    <definedName name="_xlchart.v1.135" hidden="1">results1!$A$21:$LS$21</definedName>
+    <definedName name="_xlchart.v1.136" hidden="1">results1!$A$22:$LS$22</definedName>
+    <definedName name="_xlchart.v1.137" hidden="1">results1!$A$23:$LS$23</definedName>
+    <definedName name="_xlchart.v1.138" hidden="1">results1!$A$24:$LS$24</definedName>
+    <definedName name="_xlchart.v1.139" hidden="1">results1!$A$25:$LS$25</definedName>
     <definedName name="_xlchart.v1.14" hidden="1">results1!$A$23:$LS$23</definedName>
+    <definedName name="_xlchart.v1.140" hidden="1">results1!$A$26:$LS$26</definedName>
+    <definedName name="_xlchart.v1.141" hidden="1">results1!$A$27:$LS$27</definedName>
+    <definedName name="_xlchart.v1.142" hidden="1">results1!$A$28:$LS$28</definedName>
+    <definedName name="_xlchart.v1.143" hidden="1">results1!$A$29:$LS$29</definedName>
+    <definedName name="_xlchart.v1.144" hidden="1">results1!$A$2:$LS$2</definedName>
+    <definedName name="_xlchart.v1.145" hidden="1">results1!$A$30:$LS$30</definedName>
+    <definedName name="_xlchart.v1.146" hidden="1">results1!$A$3:$LS$3</definedName>
+    <definedName name="_xlchart.v1.147" hidden="1">results1!$A$4:$LS$4</definedName>
+    <definedName name="_xlchart.v1.148" hidden="1">results1!$A$5:$LS$5</definedName>
+    <definedName name="_xlchart.v1.149" hidden="1">results1!$A$6:$LS$6</definedName>
     <definedName name="_xlchart.v1.15" hidden="1">results1!$A$24:$LS$24</definedName>
+    <definedName name="_xlchart.v1.150" hidden="1">results1!$A$7:$LS$7</definedName>
+    <definedName name="_xlchart.v1.151" hidden="1">results1!$A$8:$LS$8</definedName>
+    <definedName name="_xlchart.v1.152" hidden="1">results1!$A$9:$LS$9</definedName>
+    <definedName name="_xlchart.v1.153" hidden="1">results1!$A$9:$LS$9</definedName>
+    <definedName name="_xlchart.v1.154" hidden="1">results1!$A$10:$LS$10</definedName>
+    <definedName name="_xlchart.v1.155" hidden="1">results1!$A$11:$LS$11</definedName>
+    <definedName name="_xlchart.v1.156" hidden="1">results1!$A$12:$LS$12</definedName>
+    <definedName name="_xlchart.v1.157" hidden="1">results1!$A$13:$LS$13</definedName>
+    <definedName name="_xlchart.v1.158" hidden="1">results1!$A$14:$LS$14</definedName>
+    <definedName name="_xlchart.v1.159" hidden="1">results1!$A$15:$LS$15</definedName>
     <definedName name="_xlchart.v1.16" hidden="1">results1!$A$25:$LS$25</definedName>
+    <definedName name="_xlchart.v1.160" hidden="1">results1!$A$16:$LS$16</definedName>
+    <definedName name="_xlchart.v1.161" hidden="1">results1!$A$17:$LS$17</definedName>
+    <definedName name="_xlchart.v1.162" hidden="1">results1!$A$18:$LS$18</definedName>
+    <definedName name="_xlchart.v1.163" hidden="1">results1!$A$19:$LS$19</definedName>
+    <definedName name="_xlchart.v1.164" hidden="1">results1!$A$1:$LS$1</definedName>
+    <definedName name="_xlchart.v1.165" hidden="1">results1!$A$20:$LS$20</definedName>
+    <definedName name="_xlchart.v1.166" hidden="1">results1!$A$21:$LS$21</definedName>
+    <definedName name="_xlchart.v1.167" hidden="1">results1!$A$22:$LS$22</definedName>
+    <definedName name="_xlchart.v1.168" hidden="1">results1!$A$23:$LS$23</definedName>
+    <definedName name="_xlchart.v1.169" hidden="1">results1!$A$24:$LS$24</definedName>
     <definedName name="_xlchart.v1.17" hidden="1">results1!$A$26:$LS$26</definedName>
+    <definedName name="_xlchart.v1.170" hidden="1">results1!$A$25:$LS$25</definedName>
+    <definedName name="_xlchart.v1.171" hidden="1">results1!$A$26:$LS$26</definedName>
+    <definedName name="_xlchart.v1.172" hidden="1">results1!$A$27:$LS$27</definedName>
+    <definedName name="_xlchart.v1.173" hidden="1">results1!$A$28:$LS$28</definedName>
+    <definedName name="_xlchart.v1.174" hidden="1">results1!$A$29:$LS$29</definedName>
+    <definedName name="_xlchart.v1.175" hidden="1">results1!$A$2:$LS$2</definedName>
+    <definedName name="_xlchart.v1.176" hidden="1">results1!$A$30:$LS$30</definedName>
+    <definedName name="_xlchart.v1.177" hidden="1">results1!$A$3:$LS$3</definedName>
+    <definedName name="_xlchart.v1.178" hidden="1">results1!$A$4:$LS$4</definedName>
+    <definedName name="_xlchart.v1.179" hidden="1">results1!$A$5:$LS$5</definedName>
     <definedName name="_xlchart.v1.18" hidden="1">results1!$A$27:$LS$27</definedName>
+    <definedName name="_xlchart.v1.180" hidden="1">results1!$A$6:$LS$6</definedName>
+    <definedName name="_xlchart.v1.181" hidden="1">results1!$A$7:$LS$7</definedName>
+    <definedName name="_xlchart.v1.182" hidden="1">results1!$A$8:$LS$8</definedName>
+    <definedName name="_xlchart.v1.183" hidden="1">results1!$A$9:$LS$9</definedName>
+    <definedName name="_xlchart.v1.184" hidden="1">results1!$A$9:$LS$9</definedName>
+    <definedName name="_xlchart.v1.185" hidden="1">results1!$A$10:$LS$10</definedName>
+    <definedName name="_xlchart.v1.186" hidden="1">results1!$A$11:$LS$11</definedName>
+    <definedName name="_xlchart.v1.187" hidden="1">results1!$A$12:$LS$12</definedName>
+    <definedName name="_xlchart.v1.188" hidden="1">results1!$A$13:$LS$13</definedName>
+    <definedName name="_xlchart.v1.189" hidden="1">results1!$A$14:$LS$14</definedName>
     <definedName name="_xlchart.v1.19" hidden="1">results1!$A$28:$LS$28</definedName>
+    <definedName name="_xlchart.v1.190" hidden="1">results1!$A$15:$LS$15</definedName>
+    <definedName name="_xlchart.v1.191" hidden="1">results1!$A$16:$LS$16</definedName>
+    <definedName name="_xlchart.v1.192" hidden="1">results1!$A$17:$LS$17</definedName>
+    <definedName name="_xlchart.v1.193" hidden="1">results1!$A$18:$LS$18</definedName>
+    <definedName name="_xlchart.v1.194" hidden="1">results1!$A$19:$LS$19</definedName>
+    <definedName name="_xlchart.v1.195" hidden="1">results1!$A$1:$LS$1</definedName>
+    <definedName name="_xlchart.v1.196" hidden="1">results1!$A$20:$LS$20</definedName>
+    <definedName name="_xlchart.v1.197" hidden="1">results1!$A$21:$LS$21</definedName>
+    <definedName name="_xlchart.v1.198" hidden="1">results1!$A$22:$LS$22</definedName>
+    <definedName name="_xlchart.v1.199" hidden="1">results1!$A$23:$LS$23</definedName>
     <definedName name="_xlchart.v1.2" hidden="1">results1!$A$12:$LS$12</definedName>
     <definedName name="_xlchart.v1.20" hidden="1">results1!$A$29:$LS$29</definedName>
+    <definedName name="_xlchart.v1.200" hidden="1">results1!$A$24:$LS$24</definedName>
+    <definedName name="_xlchart.v1.201" hidden="1">results1!$A$25:$LS$25</definedName>
+    <definedName name="_xlchart.v1.202" hidden="1">results1!$A$26:$LS$26</definedName>
+    <definedName name="_xlchart.v1.203" hidden="1">results1!$A$27:$LS$27</definedName>
+    <definedName name="_xlchart.v1.204" hidden="1">results1!$A$28:$LS$28</definedName>
+    <definedName name="_xlchart.v1.205" hidden="1">results1!$A$29:$LS$29</definedName>
+    <definedName name="_xlchart.v1.206" hidden="1">results1!$A$2:$LS$2</definedName>
+    <definedName name="_xlchart.v1.207" hidden="1">results1!$A$30:$LS$30</definedName>
+    <definedName name="_xlchart.v1.208" hidden="1">results1!$A$3:$LS$3</definedName>
+    <definedName name="_xlchart.v1.209" hidden="1">results1!$A$4:$LS$4</definedName>
     <definedName name="_xlchart.v1.21" hidden="1">results1!$A$2:$LS$2</definedName>
+    <definedName name="_xlchart.v1.210" hidden="1">results1!$A$5:$LS$5</definedName>
+    <definedName name="_xlchart.v1.211" hidden="1">results1!$A$6:$LS$6</definedName>
+    <definedName name="_xlchart.v1.212" hidden="1">results1!$A$7:$LS$7</definedName>
+    <definedName name="_xlchart.v1.213" hidden="1">results1!$A$8:$LS$8</definedName>
+    <definedName name="_xlchart.v1.214" hidden="1">results1!$A$9:$LS$9</definedName>
+    <definedName name="_xlchart.v1.215" hidden="1">results1!$A$9:$LS$9</definedName>
+    <definedName name="_xlchart.v1.216" hidden="1">results1!$A$10:$LS$10</definedName>
+    <definedName name="_xlchart.v1.217" hidden="1">results1!$A$11:$LS$11</definedName>
+    <definedName name="_xlchart.v1.218" hidden="1">results1!$A$12:$LS$12</definedName>
+    <definedName name="_xlchart.v1.219" hidden="1">results1!$A$13:$LS$13</definedName>
     <definedName name="_xlchart.v1.22" hidden="1">results1!$A$30:$LS$30</definedName>
+    <definedName name="_xlchart.v1.220" hidden="1">results1!$A$14:$LS$14</definedName>
+    <definedName name="_xlchart.v1.221" hidden="1">results1!$A$15:$LS$15</definedName>
+    <definedName name="_xlchart.v1.222" hidden="1">results1!$A$16:$LS$16</definedName>
+    <definedName name="_xlchart.v1.223" hidden="1">results1!$A$17:$LS$17</definedName>
+    <definedName name="_xlchart.v1.224" hidden="1">results1!$A$18:$LS$18</definedName>
+    <definedName name="_xlchart.v1.225" hidden="1">results1!$A$19:$LS$19</definedName>
+    <definedName name="_xlchart.v1.226" hidden="1">results1!$A$1:$LS$1</definedName>
+    <definedName name="_xlchart.v1.227" hidden="1">results1!$A$20:$LS$20</definedName>
+    <definedName name="_xlchart.v1.228" hidden="1">results1!$A$21:$LS$21</definedName>
+    <definedName name="_xlchart.v1.229" hidden="1">results1!$A$22:$LS$22</definedName>
     <definedName name="_xlchart.v1.23" hidden="1">results1!$A$3:$LS$3</definedName>
+    <definedName name="_xlchart.v1.230" hidden="1">results1!$A$23:$LS$23</definedName>
+    <definedName name="_xlchart.v1.231" hidden="1">results1!$A$24:$LS$24</definedName>
+    <definedName name="_xlchart.v1.232" hidden="1">results1!$A$25:$LS$25</definedName>
+    <definedName name="_xlchart.v1.233" hidden="1">results1!$A$26:$LS$26</definedName>
+    <definedName name="_xlchart.v1.234" hidden="1">results1!$A$27:$LS$27</definedName>
+    <definedName name="_xlchart.v1.235" hidden="1">results1!$A$28:$LS$28</definedName>
+    <definedName name="_xlchart.v1.236" hidden="1">results1!$A$29:$LS$29</definedName>
+    <definedName name="_xlchart.v1.237" hidden="1">results1!$A$2:$LS$2</definedName>
+    <definedName name="_xlchart.v1.238" hidden="1">results1!$A$30:$LS$30</definedName>
+    <definedName name="_xlchart.v1.239" hidden="1">results1!$A$3:$LS$3</definedName>
     <definedName name="_xlchart.v1.24" hidden="1">results1!$A$4:$LS$4</definedName>
+    <definedName name="_xlchart.v1.240" hidden="1">results1!$A$4:$LS$4</definedName>
+    <definedName name="_xlchart.v1.241" hidden="1">results1!$A$5:$LS$5</definedName>
+    <definedName name="_xlchart.v1.242" hidden="1">results1!$A$6:$LS$6</definedName>
+    <definedName name="_xlchart.v1.243" hidden="1">results1!$A$7:$LS$7</definedName>
+    <definedName name="_xlchart.v1.244" hidden="1">results1!$A$8:$LS$8</definedName>
+    <definedName name="_xlchart.v1.245" hidden="1">results1!$A$9:$LS$9</definedName>
+    <definedName name="_xlchart.v1.246" hidden="1">results1!$A$9:$LS$9</definedName>
     <definedName name="_xlchart.v1.25" hidden="1">results1!$A$5:$LS$5</definedName>
     <definedName name="_xlchart.v1.26" hidden="1">results1!$A$6:$LS$6</definedName>
     <definedName name="_xlchart.v1.27" hidden="1">results1!$A$7:$LS$7</definedName>
@@ -92,49 +219,49 @@
     <definedName name="_xlchart.v1.58" hidden="1">results1!$A$8:$LS$8</definedName>
     <definedName name="_xlchart.v1.59" hidden="1">results1!$A$9:$LS$9</definedName>
     <definedName name="_xlchart.v1.6" hidden="1">results1!$A$16:$LS$16</definedName>
-    <definedName name="_xlchart.v1.60" hidden="1">results1!$A$10:$LS$10</definedName>
-    <definedName name="_xlchart.v1.61" hidden="1">results1!$A$11:$LS$11</definedName>
-    <definedName name="_xlchart.v1.62" hidden="1">results1!$A$12:$LS$12</definedName>
-    <definedName name="_xlchart.v1.63" hidden="1">results1!$A$13:$LS$13</definedName>
-    <definedName name="_xlchart.v1.64" hidden="1">results1!$A$14:$LS$14</definedName>
-    <definedName name="_xlchart.v1.65" hidden="1">results1!$A$15:$LS$15</definedName>
-    <definedName name="_xlchart.v1.66" hidden="1">results1!$A$16:$LS$16</definedName>
-    <definedName name="_xlchart.v1.67" hidden="1">results1!$A$17:$LS$17</definedName>
-    <definedName name="_xlchart.v1.68" hidden="1">results1!$A$18:$LS$18</definedName>
-    <definedName name="_xlchart.v1.69" hidden="1">results1!$A$19:$LS$19</definedName>
+    <definedName name="_xlchart.v1.60" hidden="1">results1!$A$9:$LS$9</definedName>
+    <definedName name="_xlchart.v1.61" hidden="1">results1!$A$10:$LS$10</definedName>
+    <definedName name="_xlchart.v1.62" hidden="1">results1!$A$11:$LS$11</definedName>
+    <definedName name="_xlchart.v1.63" hidden="1">results1!$A$12:$LS$12</definedName>
+    <definedName name="_xlchart.v1.64" hidden="1">results1!$A$13:$LS$13</definedName>
+    <definedName name="_xlchart.v1.65" hidden="1">results1!$A$14:$LS$14</definedName>
+    <definedName name="_xlchart.v1.66" hidden="1">results1!$A$15:$LS$15</definedName>
+    <definedName name="_xlchart.v1.67" hidden="1">results1!$A$16:$LS$16</definedName>
+    <definedName name="_xlchart.v1.68" hidden="1">results1!$A$17:$LS$17</definedName>
+    <definedName name="_xlchart.v1.69" hidden="1">results1!$A$18:$LS$18</definedName>
     <definedName name="_xlchart.v1.7" hidden="1">results1!$A$17:$LS$17</definedName>
-    <definedName name="_xlchart.v1.70" hidden="1">results1!$A$1:$LS$1</definedName>
-    <definedName name="_xlchart.v1.71" hidden="1">results1!$A$20:$LS$20</definedName>
-    <definedName name="_xlchart.v1.72" hidden="1">results1!$A$21:$LS$21</definedName>
-    <definedName name="_xlchart.v1.73" hidden="1">results1!$A$22:$LS$22</definedName>
-    <definedName name="_xlchart.v1.74" hidden="1">results1!$A$23:$LS$23</definedName>
-    <definedName name="_xlchart.v1.75" hidden="1">results1!$A$24:$LS$24</definedName>
-    <definedName name="_xlchart.v1.76" hidden="1">results1!$A$25:$LS$25</definedName>
-    <definedName name="_xlchart.v1.77" hidden="1">results1!$A$26:$LS$26</definedName>
-    <definedName name="_xlchart.v1.78" hidden="1">results1!$A$27:$LS$27</definedName>
-    <definedName name="_xlchart.v1.79" hidden="1">results1!$A$28:$LS$28</definedName>
+    <definedName name="_xlchart.v1.70" hidden="1">results1!$A$19:$LS$19</definedName>
+    <definedName name="_xlchart.v1.71" hidden="1">results1!$A$1:$LS$1</definedName>
+    <definedName name="_xlchart.v1.72" hidden="1">results1!$A$20:$LS$20</definedName>
+    <definedName name="_xlchart.v1.73" hidden="1">results1!$A$21:$LS$21</definedName>
+    <definedName name="_xlchart.v1.74" hidden="1">results1!$A$22:$LS$22</definedName>
+    <definedName name="_xlchart.v1.75" hidden="1">results1!$A$23:$LS$23</definedName>
+    <definedName name="_xlchart.v1.76" hidden="1">results1!$A$24:$LS$24</definedName>
+    <definedName name="_xlchart.v1.77" hidden="1">results1!$A$25:$LS$25</definedName>
+    <definedName name="_xlchart.v1.78" hidden="1">results1!$A$26:$LS$26</definedName>
+    <definedName name="_xlchart.v1.79" hidden="1">results1!$A$27:$LS$27</definedName>
     <definedName name="_xlchart.v1.8" hidden="1">results1!$A$18:$LS$18</definedName>
-    <definedName name="_xlchart.v1.80" hidden="1">results1!$A$29:$LS$29</definedName>
-    <definedName name="_xlchart.v1.81" hidden="1">results1!$A$2:$LS$2</definedName>
-    <definedName name="_xlchart.v1.82" hidden="1">results1!$A$30:$LS$30</definedName>
-    <definedName name="_xlchart.v1.83" hidden="1">results1!$A$3:$LS$3</definedName>
-    <definedName name="_xlchart.v1.84" hidden="1">results1!$A$4:$LS$4</definedName>
-    <definedName name="_xlchart.v1.85" hidden="1">results1!$A$5:$LS$5</definedName>
-    <definedName name="_xlchart.v1.86" hidden="1">results1!$A$6:$LS$6</definedName>
-    <definedName name="_xlchart.v1.87" hidden="1">results1!$A$7:$LS$7</definedName>
-    <definedName name="_xlchart.v1.88" hidden="1">results1!$A$8:$LS$8</definedName>
-    <definedName name="_xlchart.v1.89" hidden="1">results1!$A$9:$LS$9</definedName>
+    <definedName name="_xlchart.v1.80" hidden="1">results1!$A$28:$LS$28</definedName>
+    <definedName name="_xlchart.v1.81" hidden="1">results1!$A$29:$LS$29</definedName>
+    <definedName name="_xlchart.v1.82" hidden="1">results1!$A$2:$LS$2</definedName>
+    <definedName name="_xlchart.v1.83" hidden="1">results1!$A$30:$LS$30</definedName>
+    <definedName name="_xlchart.v1.84" hidden="1">results1!$A$3:$LS$3</definedName>
+    <definedName name="_xlchart.v1.85" hidden="1">results1!$A$4:$LS$4</definedName>
+    <definedName name="_xlchart.v1.86" hidden="1">results1!$A$5:$LS$5</definedName>
+    <definedName name="_xlchart.v1.87" hidden="1">results1!$A$6:$LS$6</definedName>
+    <definedName name="_xlchart.v1.88" hidden="1">results1!$A$7:$LS$7</definedName>
+    <definedName name="_xlchart.v1.89" hidden="1">results1!$A$8:$LS$8</definedName>
     <definedName name="_xlchart.v1.9" hidden="1">results1!$A$19:$LS$19</definedName>
-    <definedName name="_xlchart.v1.90" hidden="1">results1!$A$10:$LS$10</definedName>
-    <definedName name="_xlchart.v1.91" hidden="1">results1!$A$11:$LS$11</definedName>
-    <definedName name="_xlchart.v1.92" hidden="1">results1!$A$12:$LS$12</definedName>
-    <definedName name="_xlchart.v1.93" hidden="1">results1!$A$13:$LS$13</definedName>
-    <definedName name="_xlchart.v1.94" hidden="1">results1!$A$14:$LS$14</definedName>
-    <definedName name="_xlchart.v1.95" hidden="1">results1!$A$15:$LS$15</definedName>
-    <definedName name="_xlchart.v1.96" hidden="1">results1!$A$16:$LS$16</definedName>
-    <definedName name="_xlchart.v1.97" hidden="1">results1!$A$17:$LS$17</definedName>
-    <definedName name="_xlchart.v1.98" hidden="1">results1!$A$18:$LS$18</definedName>
-    <definedName name="_xlchart.v1.99" hidden="1">results1!$A$19:$LS$19</definedName>
+    <definedName name="_xlchart.v1.90" hidden="1">results1!$A$9:$LS$9</definedName>
+    <definedName name="_xlchart.v1.91" hidden="1">results1!$A$9:$LS$9</definedName>
+    <definedName name="_xlchart.v1.92" hidden="1">results1!$A$10:$LS$10</definedName>
+    <definedName name="_xlchart.v1.93" hidden="1">results1!$A$11:$LS$11</definedName>
+    <definedName name="_xlchart.v1.94" hidden="1">results1!$A$12:$LS$12</definedName>
+    <definedName name="_xlchart.v1.95" hidden="1">results1!$A$13:$LS$13</definedName>
+    <definedName name="_xlchart.v1.96" hidden="1">results1!$A$14:$LS$14</definedName>
+    <definedName name="_xlchart.v1.97" hidden="1">results1!$A$15:$LS$15</definedName>
+    <definedName name="_xlchart.v1.98" hidden="1">results1!$A$16:$LS$16</definedName>
+    <definedName name="_xlchart.v1.99" hidden="1">results1!$A$17:$LS$17</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
@@ -668,6 +795,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFBD5600"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -684,192 +816,167 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:numDim type="val">
-        <cx:f dir="row">_xlchart.v1.100</cx:f>
+        <cx:f dir="row">_xlchart.v1.10</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="1">
       <cx:numDim type="val">
-        <cx:f dir="row">_xlchart.v1.111</cx:f>
+        <cx:f dir="row">_xlchart.v1.21</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="2">
       <cx:numDim type="val">
-        <cx:f dir="row">_xlchart.v1.113</cx:f>
+        <cx:f dir="row">_xlchart.v1.23</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="3">
       <cx:numDim type="val">
-        <cx:f dir="row">_xlchart.v1.114</cx:f>
+        <cx:f dir="row">_xlchart.v1.24</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="4">
       <cx:numDim type="val">
-        <cx:f dir="row">_xlchart.v1.115</cx:f>
+        <cx:f dir="row">_xlchart.v1.25</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="5">
       <cx:numDim type="val">
-        <cx:f dir="row">_xlchart.v1.116</cx:f>
+        <cx:f dir="row">_xlchart.v1.26</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="6">
       <cx:numDim type="val">
-        <cx:f dir="row">_xlchart.v1.117</cx:f>
+        <cx:f dir="row">_xlchart.v1.27</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="7">
       <cx:numDim type="val">
-        <cx:f dir="row">_xlchart.v1.118</cx:f>
+        <cx:f dir="row">_xlchart.v1.28</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="8">
       <cx:numDim type="val">
-        <cx:f dir="row">_xlchart.v1.119</cx:f>
+        <cx:f dir="row">_xlchart.v1.29</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="9">
       <cx:numDim type="val">
-        <cx:f dir="row">_xlchart.v1.90</cx:f>
+        <cx:f dir="row">_xlchart.v1.0</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="10">
       <cx:numDim type="val">
-        <cx:f dir="row">_xlchart.v1.91</cx:f>
+        <cx:f dir="row">_xlchart.v1.1</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="11">
       <cx:numDim type="val">
-        <cx:f dir="row">_xlchart.v1.92</cx:f>
+        <cx:f dir="row">_xlchart.v1.2</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="12">
       <cx:numDim type="val">
-        <cx:f dir="row">_xlchart.v1.93</cx:f>
+        <cx:f dir="row">_xlchart.v1.3</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="13">
       <cx:numDim type="val">
-        <cx:f dir="row">_xlchart.v1.94</cx:f>
+        <cx:f dir="row">_xlchart.v1.4</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="14">
       <cx:numDim type="val">
-        <cx:f dir="row">_xlchart.v1.95</cx:f>
+        <cx:f dir="row">_xlchart.v1.5</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="15">
       <cx:numDim type="val">
-        <cx:f dir="row">_xlchart.v1.96</cx:f>
+        <cx:f dir="row">_xlchart.v1.6</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="16">
       <cx:numDim type="val">
-        <cx:f dir="row">_xlchart.v1.97</cx:f>
+        <cx:f dir="row">_xlchart.v1.7</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="17">
       <cx:numDim type="val">
-        <cx:f dir="row">_xlchart.v1.98</cx:f>
+        <cx:f dir="row">_xlchart.v1.8</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="18">
       <cx:numDim type="val">
-        <cx:f dir="row">_xlchart.v1.99</cx:f>
+        <cx:f dir="row">_xlchart.v1.9</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="19">
       <cx:numDim type="val">
-        <cx:f dir="row">_xlchart.v1.101</cx:f>
+        <cx:f dir="row">_xlchart.v1.11</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="20">
       <cx:numDim type="val">
-        <cx:f dir="row">_xlchart.v1.102</cx:f>
+        <cx:f dir="row">_xlchart.v1.12</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="21">
       <cx:numDim type="val">
-        <cx:f dir="row">_xlchart.v1.103</cx:f>
+        <cx:f dir="row">_xlchart.v1.13</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="22">
       <cx:numDim type="val">
-        <cx:f dir="row">_xlchart.v1.104</cx:f>
+        <cx:f dir="row">_xlchart.v1.14</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="23">
       <cx:numDim type="val">
-        <cx:f dir="row">_xlchart.v1.105</cx:f>
+        <cx:f dir="row">_xlchart.v1.15</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="24">
       <cx:numDim type="val">
-        <cx:f dir="row">_xlchart.v1.106</cx:f>
+        <cx:f dir="row">_xlchart.v1.16</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="25">
       <cx:numDim type="val">
-        <cx:f dir="row">_xlchart.v1.107</cx:f>
+        <cx:f dir="row">_xlchart.v1.17</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="26">
       <cx:numDim type="val">
-        <cx:f dir="row">_xlchart.v1.108</cx:f>
+        <cx:f dir="row">_xlchart.v1.18</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="27">
       <cx:numDim type="val">
-        <cx:f dir="row">_xlchart.v1.109</cx:f>
+        <cx:f dir="row">_xlchart.v1.19</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="28">
       <cx:numDim type="val">
-        <cx:f dir="row">_xlchart.v1.110</cx:f>
+        <cx:f dir="row">_xlchart.v1.20</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="29">
       <cx:numDim type="val">
-        <cx:f dir="row">_xlchart.v1.112</cx:f>
+        <cx:f dir="row">_xlchart.v1.22</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
   <cx:chart>
-    <cx:title pos="t" align="ctr" overlay="0">
-      <cx:tx>
-        <cx:txData>
-          <cx:v>Histogram of Travel Times</cx:v>
-        </cx:txData>
-      </cx:tx>
-      <cx:txPr>
-        <a:bodyPr spcFirstLastPara="1" vertOverflow="ellipsis" horzOverflow="overflow" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="ctr" rtl="0">
-            <a:defRPr/>
-          </a:pPr>
-          <a:r>
-            <a:rPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0">
-              <a:solidFill>
-                <a:sysClr val="windowText" lastClr="000000">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:sysClr>
-              </a:solidFill>
-              <a:latin typeface="Calibri" panose="020F0502020204030204"/>
-            </a:rPr>
-            <a:t>Histogram of Travel Times</a:t>
-          </a:r>
-        </a:p>
-      </cx:txPr>
-    </cx:title>
     <cx:plotArea>
       <cx:plotAreaRegion>
         <cx:series layoutId="clusteredColumn" uniqueId="{E9275340-9A45-42EE-8616-54CE91AB2A39}" formatIdx="0">
+          <cx:spPr>
+            <a:solidFill>
+              <a:srgbClr val="BD5600"/>
+            </a:solidFill>
+          </cx:spPr>
           <cx:dataId val="0"/>
           <cx:layoutPr>
-            <cx:binning intervalClosed="r" underflow="auto">
-              <cx:binSize val="700"/>
-            </cx:binning>
+            <cx:binning intervalClosed="r" underflow="auto"/>
           </cx:layoutPr>
         </cx:series>
         <cx:series layoutId="clusteredColumn" hidden="1" uniqueId="{AAAA2ECE-DDE3-4460-920F-B9A80D2D1414}" formatIdx="1">
@@ -1053,6 +1160,34 @@
       </cx:axis>
       <cx:axis id="1">
         <cx:valScaling/>
+        <cx:title>
+          <cx:tx>
+            <cx:txData>
+              <cx:v>Frequency</cx:v>
+            </cx:txData>
+          </cx:tx>
+          <cx:txPr>
+            <a:bodyPr spcFirstLastPara="1" vertOverflow="ellipsis" horzOverflow="overflow" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="ctr" rtl="0">
+                <a:defRPr/>
+              </a:pPr>
+              <a:r>
+                <a:rPr lang="en-US" sz="900" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                  <a:solidFill>
+                    <a:sysClr val="windowText" lastClr="000000">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:sysClr>
+                  </a:solidFill>
+                  <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+                </a:rPr>
+                <a:t>Frequency</a:t>
+              </a:r>
+            </a:p>
+          </cx:txPr>
+        </cx:title>
         <cx:majorGridlines/>
         <cx:tickLabels/>
       </cx:axis>
@@ -1619,14 +1754,14 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>5</xdr:row>
+      <xdr:colOff>95250</xdr:colOff>
+      <xdr:row>4</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>19</xdr:row>
+      <xdr:colOff>577850</xdr:colOff>
+      <xdr:row>18</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -1663,8 +1798,8 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="609600" y="952500"/>
-              <a:ext cx="4572000" cy="2743200"/>
+              <a:off x="704850" y="736600"/>
+              <a:ext cx="4749800" cy="2654300"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -2000,9 +2135,9 @@
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:331" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:331" x14ac:dyDescent="0.35">
       <c r="A1">
         <v>1973</v>
       </c>
@@ -2997,7 +3132,7 @@
         <v>1963</v>
       </c>
     </row>
-    <row r="2" spans="1:331" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:331" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1810</v>
       </c>
@@ -3974,7 +4109,7 @@
         <v>2164</v>
       </c>
     </row>
-    <row r="3" spans="1:331" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:331" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2255</v>
       </c>
@@ -4918,7 +5053,7 @@
         <v>2243</v>
       </c>
     </row>
-    <row r="4" spans="1:331" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:331" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>2274</v>
       </c>
@@ -5838,7 +5973,7 @@
         <v>1960</v>
       </c>
     </row>
-    <row r="5" spans="1:331" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:331" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>2280</v>
       </c>
@@ -6788,7 +6923,7 @@
         <v>1922</v>
       </c>
     </row>
-    <row r="6" spans="1:331" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:331" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>1466</v>
       </c>
@@ -7669,7 +7804,7 @@
         <v>2559</v>
       </c>
     </row>
-    <row r="7" spans="1:331" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:331" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>1900</v>
       </c>
@@ -8568,7 +8703,7 @@
         <v>1964</v>
       </c>
     </row>
-    <row r="8" spans="1:331" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:331" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>2848</v>
       </c>
@@ -9455,7 +9590,7 @@
         <v>2432</v>
       </c>
     </row>
-    <row r="9" spans="1:331" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:331" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>2675</v>
       </c>
@@ -10393,7 +10528,7 @@
         <v>2292</v>
       </c>
     </row>
-    <row r="10" spans="1:331" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:331" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>2281</v>
       </c>
@@ -11367,7 +11502,7 @@
         <v>2104</v>
       </c>
     </row>
-    <row r="11" spans="1:331" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:331" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>2058</v>
       </c>
@@ -12254,7 +12389,7 @@
         <v>2181</v>
       </c>
     </row>
-    <row r="12" spans="1:331" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:331" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>2111</v>
       </c>
@@ -13150,7 +13285,7 @@
         <v>2044</v>
       </c>
     </row>
-    <row r="13" spans="1:331" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:331" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>1736</v>
       </c>
@@ -14079,7 +14214,7 @@
         <v>2041</v>
       </c>
     </row>
-    <row r="14" spans="1:331" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:331" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>1804</v>
       </c>
@@ -15035,7 +15170,7 @@
         <v>2279</v>
       </c>
     </row>
-    <row r="15" spans="1:331" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:331" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>1610</v>
       </c>
@@ -15976,7 +16111,7 @@
         <v>2309</v>
       </c>
     </row>
-    <row r="16" spans="1:331" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:331" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>1981</v>
       </c>
@@ -16854,7 +16989,7 @@
         <v>2556</v>
       </c>
     </row>
-    <row r="17" spans="1:324" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:324" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>1771</v>
       </c>
@@ -17789,7 +17924,7 @@
         <v>2680</v>
       </c>
     </row>
-    <row r="18" spans="1:324" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:324" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>2133</v>
       </c>
@@ -18718,7 +18853,7 @@
         <v>2218</v>
       </c>
     </row>
-    <row r="19" spans="1:324" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:324" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>1835</v>
       </c>
@@ -19560,7 +19695,7 @@
         <v>2547</v>
       </c>
     </row>
-    <row r="20" spans="1:324" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:324" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>1570</v>
       </c>
@@ -20486,7 +20621,7 @@
         <v>3040</v>
       </c>
     </row>
-    <row r="21" spans="1:324" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:324" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>1772</v>
       </c>
@@ -21430,7 +21565,7 @@
         <v>2216</v>
       </c>
     </row>
-    <row r="22" spans="1:324" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:324" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>1877</v>
       </c>
@@ -22329,7 +22464,7 @@
         <v>1924</v>
       </c>
     </row>
-    <row r="23" spans="1:324" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:324" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>2333</v>
       </c>
@@ -23279,7 +23414,7 @@
         <v>2092</v>
       </c>
     </row>
-    <row r="24" spans="1:324" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:324" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>1744</v>
       </c>
@@ -24235,7 +24370,7 @@
         <v>2190</v>
       </c>
     </row>
-    <row r="25" spans="1:324" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:324" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>2330</v>
       </c>
@@ -25200,7 +25335,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="26" spans="1:324" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:324" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>1822</v>
       </c>
@@ -26117,7 +26252,7 @@
         <v>2027</v>
       </c>
     </row>
-    <row r="27" spans="1:324" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:324" x14ac:dyDescent="0.35">
       <c r="A27">
         <v>2491</v>
       </c>
@@ -27055,7 +27190,7 @@
         <v>2347</v>
       </c>
     </row>
-    <row r="28" spans="1:324" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:324" x14ac:dyDescent="0.35">
       <c r="A28">
         <v>2192</v>
       </c>
@@ -27948,7 +28083,7 @@
         <v>2816</v>
       </c>
     </row>
-    <row r="29" spans="1:324" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:324" x14ac:dyDescent="0.35">
       <c r="A29">
         <v>2484</v>
       </c>
@@ -28922,7 +29057,7 @@
         <v>1878</v>
       </c>
     </row>
-    <row r="30" spans="1:324" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:324" x14ac:dyDescent="0.35">
       <c r="A30">
         <v>1585</v>
       </c>

</xml_diff>

<commit_message>
updated presentation and results
</commit_message>
<xml_diff>
--- a/results1.xlsx
+++ b/results1.xlsx
@@ -18,253 +18,50 @@
     <definedName name="_xlchart.v1.0" hidden="1">results1!$A$10:$LS$10</definedName>
     <definedName name="_xlchart.v1.1" hidden="1">results1!$A$11:$LS$11</definedName>
     <definedName name="_xlchart.v1.10" hidden="1">results1!$A$1:$LS$1</definedName>
-    <definedName name="_xlchart.v1.100" hidden="1">results1!$A$18:$LS$18</definedName>
-    <definedName name="_xlchart.v1.101" hidden="1">results1!$A$19:$LS$19</definedName>
-    <definedName name="_xlchart.v1.102" hidden="1">results1!$A$1:$LS$1</definedName>
-    <definedName name="_xlchart.v1.103" hidden="1">results1!$A$20:$LS$20</definedName>
-    <definedName name="_xlchart.v1.104" hidden="1">results1!$A$21:$LS$21</definedName>
-    <definedName name="_xlchart.v1.105" hidden="1">results1!$A$22:$LS$22</definedName>
-    <definedName name="_xlchart.v1.106" hidden="1">results1!$A$23:$LS$23</definedName>
-    <definedName name="_xlchart.v1.107" hidden="1">results1!$A$24:$LS$24</definedName>
-    <definedName name="_xlchart.v1.108" hidden="1">results1!$A$25:$LS$25</definedName>
-    <definedName name="_xlchart.v1.109" hidden="1">results1!$A$26:$LS$26</definedName>
     <definedName name="_xlchart.v1.11" hidden="1">results1!$A$20:$LS$20</definedName>
-    <definedName name="_xlchart.v1.110" hidden="1">results1!$A$27:$LS$27</definedName>
-    <definedName name="_xlchart.v1.111" hidden="1">results1!$A$28:$LS$28</definedName>
-    <definedName name="_xlchart.v1.112" hidden="1">results1!$A$29:$LS$29</definedName>
-    <definedName name="_xlchart.v1.113" hidden="1">results1!$A$2:$LS$2</definedName>
-    <definedName name="_xlchart.v1.114" hidden="1">results1!$A$30:$LS$30</definedName>
-    <definedName name="_xlchart.v1.115" hidden="1">results1!$A$3:$LS$3</definedName>
-    <definedName name="_xlchart.v1.116" hidden="1">results1!$A$4:$LS$4</definedName>
-    <definedName name="_xlchart.v1.117" hidden="1">results1!$A$5:$LS$5</definedName>
-    <definedName name="_xlchart.v1.118" hidden="1">results1!$A$6:$LS$6</definedName>
-    <definedName name="_xlchart.v1.119" hidden="1">results1!$A$7:$LS$7</definedName>
     <definedName name="_xlchart.v1.12" hidden="1">results1!$A$21:$LS$21</definedName>
-    <definedName name="_xlchart.v1.120" hidden="1">results1!$A$8:$LS$8</definedName>
-    <definedName name="_xlchart.v1.121" hidden="1">results1!$A$9:$LS$9</definedName>
-    <definedName name="_xlchart.v1.122" hidden="1">results1!$A$9:$LS$9</definedName>
-    <definedName name="_xlchart.v1.123" hidden="1">results1!$A$10:$LS$10</definedName>
-    <definedName name="_xlchart.v1.124" hidden="1">results1!$A$11:$LS$11</definedName>
-    <definedName name="_xlchart.v1.125" hidden="1">results1!$A$12:$LS$12</definedName>
-    <definedName name="_xlchart.v1.126" hidden="1">results1!$A$13:$LS$13</definedName>
-    <definedName name="_xlchart.v1.127" hidden="1">results1!$A$14:$LS$14</definedName>
-    <definedName name="_xlchart.v1.128" hidden="1">results1!$A$15:$LS$15</definedName>
-    <definedName name="_xlchart.v1.129" hidden="1">results1!$A$16:$LS$16</definedName>
     <definedName name="_xlchart.v1.13" hidden="1">results1!$A$22:$LS$22</definedName>
-    <definedName name="_xlchart.v1.130" hidden="1">results1!$A$17:$LS$17</definedName>
-    <definedName name="_xlchart.v1.131" hidden="1">results1!$A$18:$LS$18</definedName>
-    <definedName name="_xlchart.v1.132" hidden="1">results1!$A$19:$LS$19</definedName>
-    <definedName name="_xlchart.v1.133" hidden="1">results1!$A$1:$LS$1</definedName>
-    <definedName name="_xlchart.v1.134" hidden="1">results1!$A$20:$LS$20</definedName>
-    <definedName name="_xlchart.v1.135" hidden="1">results1!$A$21:$LS$21</definedName>
-    <definedName name="_xlchart.v1.136" hidden="1">results1!$A$22:$LS$22</definedName>
-    <definedName name="_xlchart.v1.137" hidden="1">results1!$A$23:$LS$23</definedName>
-    <definedName name="_xlchart.v1.138" hidden="1">results1!$A$24:$LS$24</definedName>
-    <definedName name="_xlchart.v1.139" hidden="1">results1!$A$25:$LS$25</definedName>
     <definedName name="_xlchart.v1.14" hidden="1">results1!$A$23:$LS$23</definedName>
-    <definedName name="_xlchart.v1.140" hidden="1">results1!$A$26:$LS$26</definedName>
-    <definedName name="_xlchart.v1.141" hidden="1">results1!$A$27:$LS$27</definedName>
-    <definedName name="_xlchart.v1.142" hidden="1">results1!$A$28:$LS$28</definedName>
-    <definedName name="_xlchart.v1.143" hidden="1">results1!$A$29:$LS$29</definedName>
-    <definedName name="_xlchart.v1.144" hidden="1">results1!$A$2:$LS$2</definedName>
-    <definedName name="_xlchart.v1.145" hidden="1">results1!$A$30:$LS$30</definedName>
-    <definedName name="_xlchart.v1.146" hidden="1">results1!$A$3:$LS$3</definedName>
-    <definedName name="_xlchart.v1.147" hidden="1">results1!$A$4:$LS$4</definedName>
-    <definedName name="_xlchart.v1.148" hidden="1">results1!$A$5:$LS$5</definedName>
-    <definedName name="_xlchart.v1.149" hidden="1">results1!$A$6:$LS$6</definedName>
     <definedName name="_xlchart.v1.15" hidden="1">results1!$A$24:$LS$24</definedName>
-    <definedName name="_xlchart.v1.150" hidden="1">results1!$A$7:$LS$7</definedName>
-    <definedName name="_xlchart.v1.151" hidden="1">results1!$A$8:$LS$8</definedName>
-    <definedName name="_xlchart.v1.152" hidden="1">results1!$A$9:$LS$9</definedName>
-    <definedName name="_xlchart.v1.153" hidden="1">results1!$A$9:$LS$9</definedName>
-    <definedName name="_xlchart.v1.154" hidden="1">results1!$A$10:$LS$10</definedName>
-    <definedName name="_xlchart.v1.155" hidden="1">results1!$A$11:$LS$11</definedName>
-    <definedName name="_xlchart.v1.156" hidden="1">results1!$A$12:$LS$12</definedName>
-    <definedName name="_xlchart.v1.157" hidden="1">results1!$A$13:$LS$13</definedName>
-    <definedName name="_xlchart.v1.158" hidden="1">results1!$A$14:$LS$14</definedName>
-    <definedName name="_xlchart.v1.159" hidden="1">results1!$A$15:$LS$15</definedName>
     <definedName name="_xlchart.v1.16" hidden="1">results1!$A$25:$LS$25</definedName>
-    <definedName name="_xlchart.v1.160" hidden="1">results1!$A$16:$LS$16</definedName>
-    <definedName name="_xlchart.v1.161" hidden="1">results1!$A$17:$LS$17</definedName>
-    <definedName name="_xlchart.v1.162" hidden="1">results1!$A$18:$LS$18</definedName>
-    <definedName name="_xlchart.v1.163" hidden="1">results1!$A$19:$LS$19</definedName>
-    <definedName name="_xlchart.v1.164" hidden="1">results1!$A$1:$LS$1</definedName>
-    <definedName name="_xlchart.v1.165" hidden="1">results1!$A$20:$LS$20</definedName>
-    <definedName name="_xlchart.v1.166" hidden="1">results1!$A$21:$LS$21</definedName>
-    <definedName name="_xlchart.v1.167" hidden="1">results1!$A$22:$LS$22</definedName>
-    <definedName name="_xlchart.v1.168" hidden="1">results1!$A$23:$LS$23</definedName>
-    <definedName name="_xlchart.v1.169" hidden="1">results1!$A$24:$LS$24</definedName>
     <definedName name="_xlchart.v1.17" hidden="1">results1!$A$26:$LS$26</definedName>
-    <definedName name="_xlchart.v1.170" hidden="1">results1!$A$25:$LS$25</definedName>
-    <definedName name="_xlchart.v1.171" hidden="1">results1!$A$26:$LS$26</definedName>
-    <definedName name="_xlchart.v1.172" hidden="1">results1!$A$27:$LS$27</definedName>
-    <definedName name="_xlchart.v1.173" hidden="1">results1!$A$28:$LS$28</definedName>
-    <definedName name="_xlchart.v1.174" hidden="1">results1!$A$29:$LS$29</definedName>
-    <definedName name="_xlchart.v1.175" hidden="1">results1!$A$2:$LS$2</definedName>
-    <definedName name="_xlchart.v1.176" hidden="1">results1!$A$30:$LS$30</definedName>
-    <definedName name="_xlchart.v1.177" hidden="1">results1!$A$3:$LS$3</definedName>
-    <definedName name="_xlchart.v1.178" hidden="1">results1!$A$4:$LS$4</definedName>
-    <definedName name="_xlchart.v1.179" hidden="1">results1!$A$5:$LS$5</definedName>
     <definedName name="_xlchart.v1.18" hidden="1">results1!$A$27:$LS$27</definedName>
-    <definedName name="_xlchart.v1.180" hidden="1">results1!$A$6:$LS$6</definedName>
-    <definedName name="_xlchart.v1.181" hidden="1">results1!$A$7:$LS$7</definedName>
-    <definedName name="_xlchart.v1.182" hidden="1">results1!$A$8:$LS$8</definedName>
-    <definedName name="_xlchart.v1.183" hidden="1">results1!$A$9:$LS$9</definedName>
-    <definedName name="_xlchart.v1.184" hidden="1">results1!$A$9:$LS$9</definedName>
-    <definedName name="_xlchart.v1.185" hidden="1">results1!$A$10:$LS$10</definedName>
-    <definedName name="_xlchart.v1.186" hidden="1">results1!$A$11:$LS$11</definedName>
-    <definedName name="_xlchart.v1.187" hidden="1">results1!$A$12:$LS$12</definedName>
-    <definedName name="_xlchart.v1.188" hidden="1">results1!$A$13:$LS$13</definedName>
-    <definedName name="_xlchart.v1.189" hidden="1">results1!$A$14:$LS$14</definedName>
     <definedName name="_xlchart.v1.19" hidden="1">results1!$A$28:$LS$28</definedName>
-    <definedName name="_xlchart.v1.190" hidden="1">results1!$A$15:$LS$15</definedName>
-    <definedName name="_xlchart.v1.191" hidden="1">results1!$A$16:$LS$16</definedName>
-    <definedName name="_xlchart.v1.192" hidden="1">results1!$A$17:$LS$17</definedName>
-    <definedName name="_xlchart.v1.193" hidden="1">results1!$A$18:$LS$18</definedName>
-    <definedName name="_xlchart.v1.194" hidden="1">results1!$A$19:$LS$19</definedName>
-    <definedName name="_xlchart.v1.195" hidden="1">results1!$A$1:$LS$1</definedName>
-    <definedName name="_xlchart.v1.196" hidden="1">results1!$A$20:$LS$20</definedName>
-    <definedName name="_xlchart.v1.197" hidden="1">results1!$A$21:$LS$21</definedName>
-    <definedName name="_xlchart.v1.198" hidden="1">results1!$A$22:$LS$22</definedName>
-    <definedName name="_xlchart.v1.199" hidden="1">results1!$A$23:$LS$23</definedName>
     <definedName name="_xlchart.v1.2" hidden="1">results1!$A$12:$LS$12</definedName>
     <definedName name="_xlchart.v1.20" hidden="1">results1!$A$29:$LS$29</definedName>
-    <definedName name="_xlchart.v1.200" hidden="1">results1!$A$24:$LS$24</definedName>
-    <definedName name="_xlchart.v1.201" hidden="1">results1!$A$25:$LS$25</definedName>
-    <definedName name="_xlchart.v1.202" hidden="1">results1!$A$26:$LS$26</definedName>
-    <definedName name="_xlchart.v1.203" hidden="1">results1!$A$27:$LS$27</definedName>
-    <definedName name="_xlchart.v1.204" hidden="1">results1!$A$28:$LS$28</definedName>
-    <definedName name="_xlchart.v1.205" hidden="1">results1!$A$29:$LS$29</definedName>
-    <definedName name="_xlchart.v1.206" hidden="1">results1!$A$2:$LS$2</definedName>
-    <definedName name="_xlchart.v1.207" hidden="1">results1!$A$30:$LS$30</definedName>
-    <definedName name="_xlchart.v1.208" hidden="1">results1!$A$3:$LS$3</definedName>
-    <definedName name="_xlchart.v1.209" hidden="1">results1!$A$4:$LS$4</definedName>
     <definedName name="_xlchart.v1.21" hidden="1">results1!$A$2:$LS$2</definedName>
-    <definedName name="_xlchart.v1.210" hidden="1">results1!$A$5:$LS$5</definedName>
-    <definedName name="_xlchart.v1.211" hidden="1">results1!$A$6:$LS$6</definedName>
-    <definedName name="_xlchart.v1.212" hidden="1">results1!$A$7:$LS$7</definedName>
-    <definedName name="_xlchart.v1.213" hidden="1">results1!$A$8:$LS$8</definedName>
-    <definedName name="_xlchart.v1.214" hidden="1">results1!$A$9:$LS$9</definedName>
-    <definedName name="_xlchart.v1.215" hidden="1">results1!$A$9:$LS$9</definedName>
-    <definedName name="_xlchart.v1.216" hidden="1">results1!$A$10:$LS$10</definedName>
-    <definedName name="_xlchart.v1.217" hidden="1">results1!$A$11:$LS$11</definedName>
-    <definedName name="_xlchart.v1.218" hidden="1">results1!$A$12:$LS$12</definedName>
-    <definedName name="_xlchart.v1.219" hidden="1">results1!$A$13:$LS$13</definedName>
     <definedName name="_xlchart.v1.22" hidden="1">results1!$A$30:$LS$30</definedName>
-    <definedName name="_xlchart.v1.220" hidden="1">results1!$A$14:$LS$14</definedName>
-    <definedName name="_xlchart.v1.221" hidden="1">results1!$A$15:$LS$15</definedName>
-    <definedName name="_xlchart.v1.222" hidden="1">results1!$A$16:$LS$16</definedName>
-    <definedName name="_xlchart.v1.223" hidden="1">results1!$A$17:$LS$17</definedName>
-    <definedName name="_xlchart.v1.224" hidden="1">results1!$A$18:$LS$18</definedName>
-    <definedName name="_xlchart.v1.225" hidden="1">results1!$A$19:$LS$19</definedName>
-    <definedName name="_xlchart.v1.226" hidden="1">results1!$A$1:$LS$1</definedName>
-    <definedName name="_xlchart.v1.227" hidden="1">results1!$A$20:$LS$20</definedName>
-    <definedName name="_xlchart.v1.228" hidden="1">results1!$A$21:$LS$21</definedName>
-    <definedName name="_xlchart.v1.229" hidden="1">results1!$A$22:$LS$22</definedName>
     <definedName name="_xlchart.v1.23" hidden="1">results1!$A$3:$LS$3</definedName>
-    <definedName name="_xlchart.v1.230" hidden="1">results1!$A$23:$LS$23</definedName>
-    <definedName name="_xlchart.v1.231" hidden="1">results1!$A$24:$LS$24</definedName>
-    <definedName name="_xlchart.v1.232" hidden="1">results1!$A$25:$LS$25</definedName>
-    <definedName name="_xlchart.v1.233" hidden="1">results1!$A$26:$LS$26</definedName>
-    <definedName name="_xlchart.v1.234" hidden="1">results1!$A$27:$LS$27</definedName>
-    <definedName name="_xlchart.v1.235" hidden="1">results1!$A$28:$LS$28</definedName>
-    <definedName name="_xlchart.v1.236" hidden="1">results1!$A$29:$LS$29</definedName>
-    <definedName name="_xlchart.v1.237" hidden="1">results1!$A$2:$LS$2</definedName>
-    <definedName name="_xlchart.v1.238" hidden="1">results1!$A$30:$LS$30</definedName>
-    <definedName name="_xlchart.v1.239" hidden="1">results1!$A$3:$LS$3</definedName>
     <definedName name="_xlchart.v1.24" hidden="1">results1!$A$4:$LS$4</definedName>
-    <definedName name="_xlchart.v1.240" hidden="1">results1!$A$4:$LS$4</definedName>
-    <definedName name="_xlchart.v1.241" hidden="1">results1!$A$5:$LS$5</definedName>
-    <definedName name="_xlchart.v1.242" hidden="1">results1!$A$6:$LS$6</definedName>
-    <definedName name="_xlchart.v1.243" hidden="1">results1!$A$7:$LS$7</definedName>
-    <definedName name="_xlchart.v1.244" hidden="1">results1!$A$8:$LS$8</definedName>
-    <definedName name="_xlchart.v1.245" hidden="1">results1!$A$9:$LS$9</definedName>
-    <definedName name="_xlchart.v1.246" hidden="1">results1!$A$9:$LS$9</definedName>
     <definedName name="_xlchart.v1.25" hidden="1">results1!$A$5:$LS$5</definedName>
     <definedName name="_xlchart.v1.26" hidden="1">results1!$A$6:$LS$6</definedName>
     <definedName name="_xlchart.v1.27" hidden="1">results1!$A$7:$LS$7</definedName>
     <definedName name="_xlchart.v1.28" hidden="1">results1!$A$8:$LS$8</definedName>
     <definedName name="_xlchart.v1.29" hidden="1">results1!$A$9:$LS$9</definedName>
     <definedName name="_xlchart.v1.3" hidden="1">results1!$A$13:$LS$13</definedName>
-    <definedName name="_xlchart.v1.30" hidden="1">results1!$A$10:$LS$10</definedName>
-    <definedName name="_xlchart.v1.31" hidden="1">results1!$A$11:$LS$11</definedName>
-    <definedName name="_xlchart.v1.32" hidden="1">results1!$A$12:$LS$12</definedName>
-    <definedName name="_xlchart.v1.33" hidden="1">results1!$A$13:$LS$13</definedName>
-    <definedName name="_xlchart.v1.34" hidden="1">results1!$A$14:$LS$14</definedName>
-    <definedName name="_xlchart.v1.35" hidden="1">results1!$A$15:$LS$15</definedName>
-    <definedName name="_xlchart.v1.36" hidden="1">results1!$A$16:$LS$16</definedName>
-    <definedName name="_xlchart.v1.37" hidden="1">results1!$A$17:$LS$17</definedName>
-    <definedName name="_xlchart.v1.38" hidden="1">results1!$A$18:$LS$18</definedName>
-    <definedName name="_xlchart.v1.39" hidden="1">results1!$A$19:$LS$19</definedName>
     <definedName name="_xlchart.v1.4" hidden="1">results1!$A$14:$LS$14</definedName>
-    <definedName name="_xlchart.v1.40" hidden="1">results1!$A$1:$LS$1</definedName>
-    <definedName name="_xlchart.v1.41" hidden="1">results1!$A$20:$LS$20</definedName>
-    <definedName name="_xlchart.v1.42" hidden="1">results1!$A$21:$LS$21</definedName>
-    <definedName name="_xlchart.v1.43" hidden="1">results1!$A$22:$LS$22</definedName>
-    <definedName name="_xlchart.v1.44" hidden="1">results1!$A$23:$LS$23</definedName>
-    <definedName name="_xlchart.v1.45" hidden="1">results1!$A$24:$LS$24</definedName>
-    <definedName name="_xlchart.v1.46" hidden="1">results1!$A$25:$LS$25</definedName>
-    <definedName name="_xlchart.v1.47" hidden="1">results1!$A$26:$LS$26</definedName>
-    <definedName name="_xlchart.v1.48" hidden="1">results1!$A$27:$LS$27</definedName>
-    <definedName name="_xlchart.v1.49" hidden="1">results1!$A$28:$LS$28</definedName>
     <definedName name="_xlchart.v1.5" hidden="1">results1!$A$15:$LS$15</definedName>
-    <definedName name="_xlchart.v1.50" hidden="1">results1!$A$29:$LS$29</definedName>
-    <definedName name="_xlchart.v1.51" hidden="1">results1!$A$2:$LS$2</definedName>
-    <definedName name="_xlchart.v1.52" hidden="1">results1!$A$30:$LS$30</definedName>
-    <definedName name="_xlchart.v1.53" hidden="1">results1!$A$3:$LS$3</definedName>
-    <definedName name="_xlchart.v1.54" hidden="1">results1!$A$4:$LS$4</definedName>
-    <definedName name="_xlchart.v1.55" hidden="1">results1!$A$5:$LS$5</definedName>
-    <definedName name="_xlchart.v1.56" hidden="1">results1!$A$6:$LS$6</definedName>
-    <definedName name="_xlchart.v1.57" hidden="1">results1!$A$7:$LS$7</definedName>
-    <definedName name="_xlchart.v1.58" hidden="1">results1!$A$8:$LS$8</definedName>
-    <definedName name="_xlchart.v1.59" hidden="1">results1!$A$9:$LS$9</definedName>
     <definedName name="_xlchart.v1.6" hidden="1">results1!$A$16:$LS$16</definedName>
-    <definedName name="_xlchart.v1.60" hidden="1">results1!$A$9:$LS$9</definedName>
-    <definedName name="_xlchart.v1.61" hidden="1">results1!$A$10:$LS$10</definedName>
-    <definedName name="_xlchart.v1.62" hidden="1">results1!$A$11:$LS$11</definedName>
-    <definedName name="_xlchart.v1.63" hidden="1">results1!$A$12:$LS$12</definedName>
-    <definedName name="_xlchart.v1.64" hidden="1">results1!$A$13:$LS$13</definedName>
-    <definedName name="_xlchart.v1.65" hidden="1">results1!$A$14:$LS$14</definedName>
-    <definedName name="_xlchart.v1.66" hidden="1">results1!$A$15:$LS$15</definedName>
-    <definedName name="_xlchart.v1.67" hidden="1">results1!$A$16:$LS$16</definedName>
-    <definedName name="_xlchart.v1.68" hidden="1">results1!$A$17:$LS$17</definedName>
-    <definedName name="_xlchart.v1.69" hidden="1">results1!$A$18:$LS$18</definedName>
     <definedName name="_xlchart.v1.7" hidden="1">results1!$A$17:$LS$17</definedName>
-    <definedName name="_xlchart.v1.70" hidden="1">results1!$A$19:$LS$19</definedName>
-    <definedName name="_xlchart.v1.71" hidden="1">results1!$A$1:$LS$1</definedName>
-    <definedName name="_xlchart.v1.72" hidden="1">results1!$A$20:$LS$20</definedName>
-    <definedName name="_xlchart.v1.73" hidden="1">results1!$A$21:$LS$21</definedName>
-    <definedName name="_xlchart.v1.74" hidden="1">results1!$A$22:$LS$22</definedName>
-    <definedName name="_xlchart.v1.75" hidden="1">results1!$A$23:$LS$23</definedName>
-    <definedName name="_xlchart.v1.76" hidden="1">results1!$A$24:$LS$24</definedName>
-    <definedName name="_xlchart.v1.77" hidden="1">results1!$A$25:$LS$25</definedName>
-    <definedName name="_xlchart.v1.78" hidden="1">results1!$A$26:$LS$26</definedName>
-    <definedName name="_xlchart.v1.79" hidden="1">results1!$A$27:$LS$27</definedName>
     <definedName name="_xlchart.v1.8" hidden="1">results1!$A$18:$LS$18</definedName>
-    <definedName name="_xlchart.v1.80" hidden="1">results1!$A$28:$LS$28</definedName>
-    <definedName name="_xlchart.v1.81" hidden="1">results1!$A$29:$LS$29</definedName>
-    <definedName name="_xlchart.v1.82" hidden="1">results1!$A$2:$LS$2</definedName>
-    <definedName name="_xlchart.v1.83" hidden="1">results1!$A$30:$LS$30</definedName>
-    <definedName name="_xlchart.v1.84" hidden="1">results1!$A$3:$LS$3</definedName>
-    <definedName name="_xlchart.v1.85" hidden="1">results1!$A$4:$LS$4</definedName>
-    <definedName name="_xlchart.v1.86" hidden="1">results1!$A$5:$LS$5</definedName>
-    <definedName name="_xlchart.v1.87" hidden="1">results1!$A$6:$LS$6</definedName>
-    <definedName name="_xlchart.v1.88" hidden="1">results1!$A$7:$LS$7</definedName>
-    <definedName name="_xlchart.v1.89" hidden="1">results1!$A$8:$LS$8</definedName>
     <definedName name="_xlchart.v1.9" hidden="1">results1!$A$19:$LS$19</definedName>
-    <definedName name="_xlchart.v1.90" hidden="1">results1!$A$9:$LS$9</definedName>
-    <definedName name="_xlchart.v1.91" hidden="1">results1!$A$9:$LS$9</definedName>
-    <definedName name="_xlchart.v1.92" hidden="1">results1!$A$10:$LS$10</definedName>
-    <definedName name="_xlchart.v1.93" hidden="1">results1!$A$11:$LS$11</definedName>
-    <definedName name="_xlchart.v1.94" hidden="1">results1!$A$12:$LS$12</definedName>
-    <definedName name="_xlchart.v1.95" hidden="1">results1!$A$13:$LS$13</definedName>
-    <definedName name="_xlchart.v1.96" hidden="1">results1!$A$14:$LS$14</definedName>
-    <definedName name="_xlchart.v1.97" hidden="1">results1!$A$15:$LS$15</definedName>
-    <definedName name="_xlchart.v1.98" hidden="1">results1!$A$16:$LS$16</definedName>
-    <definedName name="_xlchart.v1.99" hidden="1">results1!$A$17:$LS$17</definedName>
   </definedNames>
-  <calcPr calcId="0"/>
+  <calcPr calcId="171027"/>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+  <si>
+    <t>Bins</t>
+  </si>
+  <si>
+    <t>Labels</t>
+  </si>
+  <si>
+    <t>Freq</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -811,394 +608,443 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chartEx1.xml><?xml version="1.0" encoding="utf-8"?>
-<cx:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex">
-  <cx:chartData>
-    <cx:data id="0">
-      <cx:numDim type="val">
-        <cx:f dir="row">_xlchart.v1.10</cx:f>
-      </cx:numDim>
-    </cx:data>
-    <cx:data id="1">
-      <cx:numDim type="val">
-        <cx:f dir="row">_xlchart.v1.21</cx:f>
-      </cx:numDim>
-    </cx:data>
-    <cx:data id="2">
-      <cx:numDim type="val">
-        <cx:f dir="row">_xlchart.v1.23</cx:f>
-      </cx:numDim>
-    </cx:data>
-    <cx:data id="3">
-      <cx:numDim type="val">
-        <cx:f dir="row">_xlchart.v1.24</cx:f>
-      </cx:numDim>
-    </cx:data>
-    <cx:data id="4">
-      <cx:numDim type="val">
-        <cx:f dir="row">_xlchart.v1.25</cx:f>
-      </cx:numDim>
-    </cx:data>
-    <cx:data id="5">
-      <cx:numDim type="val">
-        <cx:f dir="row">_xlchart.v1.26</cx:f>
-      </cx:numDim>
-    </cx:data>
-    <cx:data id="6">
-      <cx:numDim type="val">
-        <cx:f dir="row">_xlchart.v1.27</cx:f>
-      </cx:numDim>
-    </cx:data>
-    <cx:data id="7">
-      <cx:numDim type="val">
-        <cx:f dir="row">_xlchart.v1.28</cx:f>
-      </cx:numDim>
-    </cx:data>
-    <cx:data id="8">
-      <cx:numDim type="val">
-        <cx:f dir="row">_xlchart.v1.29</cx:f>
-      </cx:numDim>
-    </cx:data>
-    <cx:data id="9">
-      <cx:numDim type="val">
-        <cx:f dir="row">_xlchart.v1.0</cx:f>
-      </cx:numDim>
-    </cx:data>
-    <cx:data id="10">
-      <cx:numDim type="val">
-        <cx:f dir="row">_xlchart.v1.1</cx:f>
-      </cx:numDim>
-    </cx:data>
-    <cx:data id="11">
-      <cx:numDim type="val">
-        <cx:f dir="row">_xlchart.v1.2</cx:f>
-      </cx:numDim>
-    </cx:data>
-    <cx:data id="12">
-      <cx:numDim type="val">
-        <cx:f dir="row">_xlchart.v1.3</cx:f>
-      </cx:numDim>
-    </cx:data>
-    <cx:data id="13">
-      <cx:numDim type="val">
-        <cx:f dir="row">_xlchart.v1.4</cx:f>
-      </cx:numDim>
-    </cx:data>
-    <cx:data id="14">
-      <cx:numDim type="val">
-        <cx:f dir="row">_xlchart.v1.5</cx:f>
-      </cx:numDim>
-    </cx:data>
-    <cx:data id="15">
-      <cx:numDim type="val">
-        <cx:f dir="row">_xlchart.v1.6</cx:f>
-      </cx:numDim>
-    </cx:data>
-    <cx:data id="16">
-      <cx:numDim type="val">
-        <cx:f dir="row">_xlchart.v1.7</cx:f>
-      </cx:numDim>
-    </cx:data>
-    <cx:data id="17">
-      <cx:numDim type="val">
-        <cx:f dir="row">_xlchart.v1.8</cx:f>
-      </cx:numDim>
-    </cx:data>
-    <cx:data id="18">
-      <cx:numDim type="val">
-        <cx:f dir="row">_xlchart.v1.9</cx:f>
-      </cx:numDim>
-    </cx:data>
-    <cx:data id="19">
-      <cx:numDim type="val">
-        <cx:f dir="row">_xlchart.v1.11</cx:f>
-      </cx:numDim>
-    </cx:data>
-    <cx:data id="20">
-      <cx:numDim type="val">
-        <cx:f dir="row">_xlchart.v1.12</cx:f>
-      </cx:numDim>
-    </cx:data>
-    <cx:data id="21">
-      <cx:numDim type="val">
-        <cx:f dir="row">_xlchart.v1.13</cx:f>
-      </cx:numDim>
-    </cx:data>
-    <cx:data id="22">
-      <cx:numDim type="val">
-        <cx:f dir="row">_xlchart.v1.14</cx:f>
-      </cx:numDim>
-    </cx:data>
-    <cx:data id="23">
-      <cx:numDim type="val">
-        <cx:f dir="row">_xlchart.v1.15</cx:f>
-      </cx:numDim>
-    </cx:data>
-    <cx:data id="24">
-      <cx:numDim type="val">
-        <cx:f dir="row">_xlchart.v1.16</cx:f>
-      </cx:numDim>
-    </cx:data>
-    <cx:data id="25">
-      <cx:numDim type="val">
-        <cx:f dir="row">_xlchart.v1.17</cx:f>
-      </cx:numDim>
-    </cx:data>
-    <cx:data id="26">
-      <cx:numDim type="val">
-        <cx:f dir="row">_xlchart.v1.18</cx:f>
-      </cx:numDim>
-    </cx:data>
-    <cx:data id="27">
-      <cx:numDim type="val">
-        <cx:f dir="row">_xlchart.v1.19</cx:f>
-      </cx:numDim>
-    </cx:data>
-    <cx:data id="28">
-      <cx:numDim type="val">
-        <cx:f dir="row">_xlchart.v1.20</cx:f>
-      </cx:numDim>
-    </cx:data>
-    <cx:data id="29">
-      <cx:numDim type="val">
-        <cx:f dir="row">_xlchart.v1.22</cx:f>
-      </cx:numDim>
-    </cx:data>
-  </cx:chartData>
-  <cx:chart>
-    <cx:plotArea>
-      <cx:plotAreaRegion>
-        <cx:series layoutId="clusteredColumn" uniqueId="{E9275340-9A45-42EE-8616-54CE91AB2A39}" formatIdx="0">
-          <cx:spPr>
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="stacked"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
             <a:solidFill>
               <a:srgbClr val="BD5600"/>
             </a:solidFill>
-          </cx:spPr>
-          <cx:dataId val="0"/>
-          <cx:layoutPr>
-            <cx:binning intervalClosed="r" underflow="auto"/>
-          </cx:layoutPr>
-        </cx:series>
-        <cx:series layoutId="clusteredColumn" hidden="1" uniqueId="{AAAA2ECE-DDE3-4460-920F-B9A80D2D1414}" formatIdx="1">
-          <cx:dataId val="1"/>
-          <cx:layoutPr>
-            <cx:binning intervalClosed="r"/>
-          </cx:layoutPr>
-        </cx:series>
-        <cx:series layoutId="clusteredColumn" hidden="1" uniqueId="{DBAE3E02-A4BF-423C-9091-4047AB82C8E8}" formatIdx="2">
-          <cx:dataId val="2"/>
-          <cx:layoutPr>
-            <cx:binning intervalClosed="r"/>
-          </cx:layoutPr>
-        </cx:series>
-        <cx:series layoutId="clusteredColumn" hidden="1" uniqueId="{B0FBE9EB-EEDD-41AC-8289-3E7664E929B7}" formatIdx="3">
-          <cx:dataId val="3"/>
-          <cx:layoutPr>
-            <cx:binning intervalClosed="r"/>
-          </cx:layoutPr>
-        </cx:series>
-        <cx:series layoutId="clusteredColumn" hidden="1" uniqueId="{BD2A9094-45B5-4F00-B2C1-205BB6C49F59}" formatIdx="4">
-          <cx:dataId val="4"/>
-          <cx:layoutPr>
-            <cx:binning intervalClosed="r"/>
-          </cx:layoutPr>
-        </cx:series>
-        <cx:series layoutId="clusteredColumn" hidden="1" uniqueId="{291F3830-0342-4818-941D-3ABF743FD068}" formatIdx="5">
-          <cx:dataId val="5"/>
-          <cx:layoutPr>
-            <cx:binning intervalClosed="r"/>
-          </cx:layoutPr>
-        </cx:series>
-        <cx:series layoutId="clusteredColumn" hidden="1" uniqueId="{B38F189A-3017-4739-90D2-0D97B77E708E}" formatIdx="6">
-          <cx:dataId val="6"/>
-          <cx:layoutPr>
-            <cx:binning intervalClosed="r"/>
-          </cx:layoutPr>
-        </cx:series>
-        <cx:series layoutId="clusteredColumn" hidden="1" uniqueId="{DDC4BE50-91C0-4292-A83B-52138A6D0DE9}" formatIdx="7">
-          <cx:dataId val="7"/>
-          <cx:layoutPr>
-            <cx:binning intervalClosed="r"/>
-          </cx:layoutPr>
-        </cx:series>
-        <cx:series layoutId="clusteredColumn" hidden="1" uniqueId="{42D2D923-59C3-4B81-B4F9-FA47EDD1B92D}" formatIdx="8">
-          <cx:dataId val="8"/>
-          <cx:layoutPr>
-            <cx:binning intervalClosed="r"/>
-          </cx:layoutPr>
-        </cx:series>
-        <cx:series layoutId="clusteredColumn" hidden="1" uniqueId="{4E589F4C-71C5-48AE-9976-6DA65DAB1A0F}" formatIdx="9">
-          <cx:dataId val="9"/>
-          <cx:layoutPr>
-            <cx:binning intervalClosed="r"/>
-          </cx:layoutPr>
-        </cx:series>
-        <cx:series layoutId="clusteredColumn" hidden="1" uniqueId="{E073436E-1AB8-4526-9AB4-0FDE076606EC}" formatIdx="10">
-          <cx:dataId val="10"/>
-          <cx:layoutPr>
-            <cx:binning intervalClosed="r"/>
-          </cx:layoutPr>
-        </cx:series>
-        <cx:series layoutId="clusteredColumn" hidden="1" uniqueId="{20520945-63B5-4EDC-B200-83E77CBB1F22}" formatIdx="11">
-          <cx:dataId val="11"/>
-          <cx:layoutPr>
-            <cx:binning intervalClosed="r"/>
-          </cx:layoutPr>
-        </cx:series>
-        <cx:series layoutId="clusteredColumn" hidden="1" uniqueId="{DAD3C377-73C2-43FD-B5BD-DA21A4FAC72E}" formatIdx="12">
-          <cx:dataId val="12"/>
-          <cx:layoutPr>
-            <cx:binning intervalClosed="r"/>
-          </cx:layoutPr>
-        </cx:series>
-        <cx:series layoutId="clusteredColumn" hidden="1" uniqueId="{838F3B9A-85CB-4BCD-B156-F2042FAC5C74}" formatIdx="13">
-          <cx:dataId val="13"/>
-          <cx:layoutPr>
-            <cx:binning intervalClosed="r"/>
-          </cx:layoutPr>
-        </cx:series>
-        <cx:series layoutId="clusteredColumn" hidden="1" uniqueId="{D2A1AE69-45BE-4061-8E57-4DD033F6B94D}" formatIdx="14">
-          <cx:dataId val="14"/>
-          <cx:layoutPr>
-            <cx:binning intervalClosed="r"/>
-          </cx:layoutPr>
-        </cx:series>
-        <cx:series layoutId="clusteredColumn" hidden="1" uniqueId="{B368A149-D2FD-4F4C-825C-60B572512CA4}" formatIdx="15">
-          <cx:dataId val="15"/>
-          <cx:layoutPr>
-            <cx:binning intervalClosed="r"/>
-          </cx:layoutPr>
-        </cx:series>
-        <cx:series layoutId="clusteredColumn" hidden="1" uniqueId="{B2BA2272-0528-447A-A15B-3D82DEE73134}" formatIdx="16">
-          <cx:dataId val="16"/>
-          <cx:layoutPr>
-            <cx:binning intervalClosed="r"/>
-          </cx:layoutPr>
-        </cx:series>
-        <cx:series layoutId="clusteredColumn" hidden="1" uniqueId="{A447258A-6E7D-4793-A7D6-9C025E4DF026}" formatIdx="17">
-          <cx:dataId val="17"/>
-          <cx:layoutPr>
-            <cx:binning intervalClosed="r"/>
-          </cx:layoutPr>
-        </cx:series>
-        <cx:series layoutId="clusteredColumn" hidden="1" uniqueId="{EF6DB5CD-401A-46C6-88D4-4F4BAED48AB3}" formatIdx="18">
-          <cx:dataId val="18"/>
-          <cx:layoutPr>
-            <cx:binning intervalClosed="r"/>
-          </cx:layoutPr>
-        </cx:series>
-        <cx:series layoutId="clusteredColumn" hidden="1" uniqueId="{7BC8DA09-FE8B-4775-9469-8B88D73EB7EA}" formatIdx="19">
-          <cx:dataId val="19"/>
-          <cx:layoutPr>
-            <cx:binning intervalClosed="r"/>
-          </cx:layoutPr>
-        </cx:series>
-        <cx:series layoutId="clusteredColumn" hidden="1" uniqueId="{CE1696E3-15CE-4ABA-AFF4-8B6A6291F358}" formatIdx="20">
-          <cx:dataId val="20"/>
-          <cx:layoutPr>
-            <cx:binning intervalClosed="r"/>
-          </cx:layoutPr>
-        </cx:series>
-        <cx:series layoutId="clusteredColumn" hidden="1" uniqueId="{69B21529-3FA6-4430-B049-755CFC273D81}" formatIdx="21">
-          <cx:dataId val="21"/>
-          <cx:layoutPr>
-            <cx:binning intervalClosed="r"/>
-          </cx:layoutPr>
-        </cx:series>
-        <cx:series layoutId="clusteredColumn" hidden="1" uniqueId="{E1C8A16C-A763-4326-BB47-655B630A7FDA}" formatIdx="22">
-          <cx:dataId val="22"/>
-          <cx:layoutPr>
-            <cx:binning intervalClosed="r"/>
-          </cx:layoutPr>
-        </cx:series>
-        <cx:series layoutId="clusteredColumn" hidden="1" uniqueId="{6102C02B-8103-4559-A27D-1FC844A9158D}" formatIdx="23">
-          <cx:dataId val="23"/>
-          <cx:layoutPr>
-            <cx:binning intervalClosed="r"/>
-          </cx:layoutPr>
-        </cx:series>
-        <cx:series layoutId="clusteredColumn" hidden="1" uniqueId="{1CA9DFAD-8350-4BDB-BE77-65BBB74DB969}" formatIdx="24">
-          <cx:dataId val="24"/>
-          <cx:layoutPr>
-            <cx:binning intervalClosed="r"/>
-          </cx:layoutPr>
-        </cx:series>
-        <cx:series layoutId="clusteredColumn" hidden="1" uniqueId="{836F51F5-EC21-4542-AE88-42C84D373B86}" formatIdx="25">
-          <cx:dataId val="25"/>
-          <cx:layoutPr>
-            <cx:binning intervalClosed="r"/>
-          </cx:layoutPr>
-        </cx:series>
-        <cx:series layoutId="clusteredColumn" hidden="1" uniqueId="{C5BB6B68-00AB-4E8B-ADC2-EB5C088EED59}" formatIdx="26">
-          <cx:dataId val="26"/>
-          <cx:layoutPr>
-            <cx:binning intervalClosed="r"/>
-          </cx:layoutPr>
-        </cx:series>
-        <cx:series layoutId="clusteredColumn" hidden="1" uniqueId="{9DFB81CE-32AD-426B-9AF8-B26D02F047F7}" formatIdx="27">
-          <cx:dataId val="27"/>
-          <cx:layoutPr>
-            <cx:binning intervalClosed="r"/>
-          </cx:layoutPr>
-        </cx:series>
-        <cx:series layoutId="clusteredColumn" hidden="1" uniqueId="{9FF5A1BB-45AE-4C74-BE2F-574AE9AAE2B2}" formatIdx="28">
-          <cx:dataId val="28"/>
-          <cx:layoutPr>
-            <cx:binning intervalClosed="r"/>
-          </cx:layoutPr>
-        </cx:series>
-        <cx:series layoutId="clusteredColumn" hidden="1" uniqueId="{04D7CFD0-3D44-4387-8274-68DC5A6754F6}" formatIdx="29">
-          <cx:dataId val="29"/>
-          <cx:layoutPr>
-            <cx:binning intervalClosed="r"/>
-          </cx:layoutPr>
-        </cx:series>
-      </cx:plotAreaRegion>
-      <cx:axis id="0">
-        <cx:catScaling gapWidth="0"/>
-        <cx:tickLabels/>
-      </cx:axis>
-      <cx:axis id="1">
-        <cx:valScaling/>
-        <cx:title>
-          <cx:tx>
-            <cx:txData>
-              <cx:v>Frequency</cx:v>
-            </cx:txData>
-          </cx:tx>
-          <cx:txPr>
-            <a:bodyPr spcFirstLastPara="1" vertOverflow="ellipsis" horzOverflow="overflow" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" anchor="ctr" anchorCtr="1"/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>results1!$LW$2:$LW$18</c:f>
+              <c:strCache>
+                <c:ptCount val="17"/>
+                <c:pt idx="0">
+                  <c:v>170 - 200</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>200 - 230</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>230 - 260</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>260 - 290</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>290 - 320</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>320 - 350</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>350 - 380</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>380 - 410</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>410 - 440</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>440 - 470</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>470 - 500</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>500 - 530</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>530 - 560</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>560 - 590</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>590 - 620</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>620 - 650</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>&gt;650</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>results1!$LV$2:$LV$18</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="17"/>
+                <c:pt idx="0">
+                  <c:v>421</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1687</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1990</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1279</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>705</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>493</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>408</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>414</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>404</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>395</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>413</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>336</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>164</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>28</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-0026-4064-A6A6-E5E5DB5275E3}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:overlap val="100"/>
+        <c:axId val="348219120"/>
+        <c:axId val="456869848"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="348219120"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Travel</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> Time (s)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
             <a:lstStyle/>
             <a:p>
-              <a:pPr algn="ctr" rtl="0">
-                <a:defRPr/>
-              </a:pPr>
-              <a:r>
-                <a:rPr lang="en-US" sz="900" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
-                    <a:sysClr val="windowText" lastClr="000000">
+                    <a:schemeClr val="tx1">
                       <a:lumMod val="65000"/>
                       <a:lumOff val="35000"/>
-                    </a:sysClr>
+                    </a:schemeClr>
                   </a:solidFill>
-                  <a:latin typeface="Calibri" panose="020F0502020204030204"/>
-                </a:rPr>
-                <a:t>Frequency</a:t>
-              </a:r>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
-          </cx:txPr>
-        </cx:title>
-        <cx:majorGridlines/>
-        <cx:tickLabels/>
-      </cx:axis>
-    </cx:plotArea>
-  </cx:chart>
-  <cx:printSettings>
-    <cx:headerFooter alignWithMargins="1" differentOddEven="0" differentFirst="0"/>
-    <cx:pageMargins l="0.69999999999999996" r="0.69999999999999996" t="0.75" b="0.75" header="0.29999999999999999" footer="0.29999999999999999"/>
-    <cx:pageSetup paperSize="1" firstPageNumber="1" orientation="default" blackAndWhite="0" draft="0" useFirstPageNumber="0" horizontalDpi="600" verticalDpi="600" copies="1"/>
-  </cx:printSettings>
-</cx:chartSpace>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-2700000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="456869848"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="456869848"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Frequency</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="348219120"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
 </file>
 
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1242,7 +1088,7 @@
 </file>
 
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="366">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="297">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
@@ -1253,7 +1099,7 @@
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="900"/>
+    <cs:defRPr sz="1000" kern="1200"/>
   </cs:axisTitle>
   <cs:categoryAxis>
     <cs:lnRef idx="0"/>
@@ -1276,7 +1122,7 @@
         <a:round/>
       </a:ln>
     </cs:spPr>
-    <cs:defRPr sz="900"/>
+    <cs:defRPr sz="900" kern="1200"/>
   </cs:categoryAxis>
   <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
     <cs:lnRef idx="0"/>
@@ -1299,7 +1145,7 @@
         <a:round/>
       </a:ln>
     </cs:spPr>
-    <cs:defRPr sz="1000"/>
+    <cs:defRPr sz="1000" kern="1200"/>
   </cs:chartArea>
   <cs:dataLabel>
     <cs:lnRef idx="0"/>
@@ -1307,11 +1153,11 @@
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="900"/>
+    <cs:defRPr sz="900" kern="1200"/>
   </cs:dataLabel>
   <cs:dataLabelCallout>
     <cs:lnRef idx="0"/>
@@ -1336,46 +1182,36 @@
         </a:solidFill>
       </a:ln>
     </cs:spPr>
-    <cs:defRPr sz="900"/>
+    <cs:defRPr sz="900" kern="1200"/>
     <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
       <a:spAutoFit/>
     </cs:bodyPr>
   </cs:dataLabelCallout>
   <cs:dataPoint>
     <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0">
+    <cs:fillRef idx="1">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-    </cs:spPr>
   </cs:dataPoint>
   <cs:dataPoint3D>
     <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0">
+    <cs:fillRef idx="1">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-    </cs:spPr>
   </cs:dataPoint3D>
   <cs:dataPointLine>
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="0"/>
+    <cs:fillRef idx="1"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
@@ -1390,8 +1226,10 @@
     </cs:spPr>
   </cs:dataPointLine>
   <cs:dataPointMarker>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0">
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
     <cs:effectRef idx="0"/>
@@ -1399,12 +1237,9 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
       <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="lt1"/>
+          <a:schemeClr val="phClr"/>
         </a:solidFill>
       </a:ln>
     </cs:spPr>
@@ -1414,13 +1249,13 @@
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="0"/>
+    <cs:fillRef idx="1"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="28575" cap="rnd">
+      <a:ln w="9525" cap="rnd">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
@@ -1439,38 +1274,41 @@
       </a:schemeClr>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525">
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="15000"/>
             <a:lumOff val="85000"/>
           </a:schemeClr>
         </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
-    <cs:defRPr sz="900"/>
+    <cs:defRPr sz="900" kern="1200"/>
   </cs:dataTable>
   <cs:downBar>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="dk1">
-          <a:lumMod val="65000"/>
-          <a:lumOff val="35000"/>
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
         </a:schemeClr>
       </a:solidFill>
-      <a:ln w="9525">
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="65000"/>
             <a:lumOff val="35000"/>
           </a:schemeClr>
         </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:downBar>
@@ -1519,6 +1357,12 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
   </cs:floor>
   <cs:gridlineMajor>
     <cs:lnRef idx="0"/>
@@ -1550,8 +1394,8 @@
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -1569,8 +1413,8 @@
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="75000"/>
-            <a:lumOff val="25000"/>
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -1606,7 +1450,7 @@
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="900"/>
+    <cs:defRPr sz="900" kern="1200"/>
   </cs:legend>
   <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
     <cs:lnRef idx="0"/>
@@ -1634,18 +1478,7 @@
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900"/>
+    <cs:defRPr sz="900" kern="1200"/>
   </cs:seriesAxis>
   <cs:seriesLine>
     <cs:lnRef idx="0"/>
@@ -1655,9 +1488,12 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525" cap="flat">
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:srgbClr val="D9D9D9"/>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
         </a:solidFill>
         <a:round/>
       </a:ln>
@@ -1673,7 +1509,7 @@
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="1400"/>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
   </cs:title>
   <cs:trendline>
     <cs:lnRef idx="0">
@@ -1689,7 +1525,7 @@
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:prstDash val="sysDash"/>
+        <a:prstDash val="sysDot"/>
       </a:ln>
     </cs:spPr>
   </cs:trendline>
@@ -1703,26 +1539,27 @@
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="900"/>
+    <cs:defRPr sz="900" kern="1200"/>
   </cs:trendlineLabel>
   <cs:upBar>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="lt1"/>
       </a:solidFill>
-      <a:ln w="9525">
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
           </a:schemeClr>
         </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:upBar>
@@ -1736,7 +1573,7 @@
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="900"/>
+    <cs:defRPr sz="900" kern="1200"/>
   </cs:valueAxis>
   <cs:wall>
     <cs:lnRef idx="0"/>
@@ -1745,6 +1582,12 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
   </cs:wall>
 </cs:chartStyle>
 </file>
@@ -1753,80 +1596,38 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>95250</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>324</xdr:col>
+      <xdr:colOff>225425</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>577850</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:col>331</xdr:col>
+      <xdr:colOff>530225</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" Requires="cx1">
-        <xdr:graphicFrame macro="">
-          <xdr:nvGraphicFramePr>
-            <xdr:cNvPr id="3" name="Chart 2">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AD43F1F4-CAA9-427A-80C0-2ACCDAF1AA46}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvGraphicFramePr/>
-          </xdr:nvGraphicFramePr>
-          <xdr:xfrm>
-            <a:off x="0" y="0"/>
-            <a:ext cx="0" cy="0"/>
-          </xdr:xfrm>
-          <a:graphic>
-            <a:graphicData uri="http://schemas.microsoft.com/office/drawing/2014/chartex">
-              <cx:chart xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-            </a:graphicData>
-          </a:graphic>
-        </xdr:graphicFrame>
-      </mc:Choice>
-      <mc:Fallback>
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="0" name=""/>
-            <xdr:cNvSpPr>
-              <a:spLocks noTextEdit="1"/>
-            </xdr:cNvSpPr>
-          </xdr:nvSpPr>
-          <xdr:spPr>
-            <a:xfrm>
-              <a:off x="704850" y="736600"/>
-              <a:ext cx="4749800" cy="2654300"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:solidFill>
-              <a:prstClr val="white"/>
-            </a:solidFill>
-            <a:ln w="1">
-              <a:solidFill>
-                <a:prstClr val="green"/>
-              </a:solidFill>
-            </a:ln>
-          </xdr:spPr>
-          <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" horzOverflow="clip"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:r>
-                <a:rPr lang="en-US" sz="1100"/>
-                <a:t>This chart isn't available in your version of Excel.
-Editing this shape or saving this workbook into a different file format will permanently break the chart.</a:t>
-              </a:r>
-            </a:p>
-          </xdr:txBody>
-        </xdr:sp>
-      </mc:Fallback>
-    </mc:AlternateContent>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F23D4284-D8F7-4D27-B6D9-E32F74E71A24}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -2129,15 +1930,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:LS30"/>
+  <dimension ref="A1:LW30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" topLeftCell="LF1" workbookViewId="0">
+      <selection activeCell="LN19" sqref="LN19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:331" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:335" x14ac:dyDescent="0.35">
       <c r="A1">
         <v>1973</v>
       </c>
@@ -3131,8 +2932,17 @@
       <c r="LS1">
         <v>1963</v>
       </c>
+      <c r="LU1" t="s">
+        <v>0</v>
+      </c>
+      <c r="LV1" t="s">
+        <v>2</v>
+      </c>
+      <c r="LW1" t="s">
+        <v>1</v>
+      </c>
     </row>
-    <row r="2" spans="1:331" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:335" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1810</v>
       </c>
@@ -4108,8 +3918,19 @@
       <c r="LM2">
         <v>2164</v>
       </c>
+      <c r="LU2">
+        <v>1700</v>
+      </c>
+      <c r="LV2">
+        <f>COUNTIF($A$1:$LS$30,"&gt;="&amp;LU2)-COUNTIF($A$1:$LS$30,"&gt;="&amp;LU3)</f>
+        <v>421</v>
+      </c>
+      <c r="LW2" t="str">
+        <f>LU2/10&amp;" - "&amp;LU3/10</f>
+        <v>170 - 200</v>
+      </c>
     </row>
-    <row r="3" spans="1:331" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:335" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2255</v>
       </c>
@@ -5052,8 +4873,20 @@
       <c r="LB3">
         <v>2243</v>
       </c>
+      <c r="LU3">
+        <f>LU2+300</f>
+        <v>2000</v>
+      </c>
+      <c r="LV3">
+        <f t="shared" ref="LV3:LV18" si="0">COUNTIF($A$1:$LS$30,"&gt;="&amp;LU3)-COUNTIF($A$1:$LS$30,"&gt;="&amp;LU4)</f>
+        <v>1687</v>
+      </c>
+      <c r="LW3" t="str">
+        <f t="shared" ref="LW3:LW17" si="1">LU3/10&amp;" - "&amp;LU4/10</f>
+        <v>200 - 230</v>
+      </c>
     </row>
-    <row r="4" spans="1:331" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:335" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>2274</v>
       </c>
@@ -5972,8 +5805,20 @@
       <c r="KT4">
         <v>1960</v>
       </c>
+      <c r="LU4">
+        <f t="shared" ref="LU4:LU18" si="2">LU3+300</f>
+        <v>2300</v>
+      </c>
+      <c r="LV4">
+        <f t="shared" si="0"/>
+        <v>1990</v>
+      </c>
+      <c r="LW4" t="str">
+        <f t="shared" si="1"/>
+        <v>230 - 260</v>
+      </c>
     </row>
-    <row r="5" spans="1:331" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:335" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>2280</v>
       </c>
@@ -6922,8 +6767,20 @@
       <c r="LD5">
         <v>1922</v>
       </c>
+      <c r="LU5">
+        <f t="shared" si="2"/>
+        <v>2600</v>
+      </c>
+      <c r="LV5">
+        <f t="shared" si="0"/>
+        <v>1279</v>
+      </c>
+      <c r="LW5" t="str">
+        <f t="shared" si="1"/>
+        <v>260 - 290</v>
+      </c>
     </row>
-    <row r="6" spans="1:331" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:335" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>1466</v>
       </c>
@@ -7803,8 +7660,20 @@
       <c r="KG6">
         <v>2559</v>
       </c>
+      <c r="LU6">
+        <f t="shared" si="2"/>
+        <v>2900</v>
+      </c>
+      <c r="LV6">
+        <f t="shared" si="0"/>
+        <v>705</v>
+      </c>
+      <c r="LW6" t="str">
+        <f t="shared" si="1"/>
+        <v>290 - 320</v>
+      </c>
     </row>
-    <row r="7" spans="1:331" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:335" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>1900</v>
       </c>
@@ -8702,8 +8571,20 @@
       <c r="KM7">
         <v>1964</v>
       </c>
+      <c r="LU7">
+        <f t="shared" si="2"/>
+        <v>3200</v>
+      </c>
+      <c r="LV7">
+        <f t="shared" si="0"/>
+        <v>493</v>
+      </c>
+      <c r="LW7" t="str">
+        <f t="shared" si="1"/>
+        <v>320 - 350</v>
+      </c>
     </row>
-    <row r="8" spans="1:331" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:335" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>2848</v>
       </c>
@@ -9589,8 +9470,20 @@
       <c r="KI8">
         <v>2432</v>
       </c>
+      <c r="LU8">
+        <f t="shared" si="2"/>
+        <v>3500</v>
+      </c>
+      <c r="LV8">
+        <f t="shared" si="0"/>
+        <v>408</v>
+      </c>
+      <c r="LW8" t="str">
+        <f t="shared" si="1"/>
+        <v>350 - 380</v>
+      </c>
     </row>
-    <row r="9" spans="1:331" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:335" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>2675</v>
       </c>
@@ -10527,8 +10420,20 @@
       <c r="KZ9">
         <v>2292</v>
       </c>
+      <c r="LU9">
+        <f t="shared" si="2"/>
+        <v>3800</v>
+      </c>
+      <c r="LV9">
+        <f t="shared" si="0"/>
+        <v>414</v>
+      </c>
+      <c r="LW9" t="str">
+        <f t="shared" si="1"/>
+        <v>380 - 410</v>
+      </c>
     </row>
-    <row r="10" spans="1:331" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:335" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>2281</v>
       </c>
@@ -11501,8 +11406,20 @@
       <c r="LL10">
         <v>2104</v>
       </c>
+      <c r="LU10">
+        <f t="shared" si="2"/>
+        <v>4100</v>
+      </c>
+      <c r="LV10">
+        <f t="shared" si="0"/>
+        <v>404</v>
+      </c>
+      <c r="LW10" t="str">
+        <f t="shared" si="1"/>
+        <v>410 - 440</v>
+      </c>
     </row>
-    <row r="11" spans="1:331" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:335" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>2058</v>
       </c>
@@ -12388,8 +12305,20 @@
       <c r="KI11">
         <v>2181</v>
       </c>
+      <c r="LU11">
+        <f t="shared" si="2"/>
+        <v>4400</v>
+      </c>
+      <c r="LV11">
+        <f t="shared" si="0"/>
+        <v>395</v>
+      </c>
+      <c r="LW11" t="str">
+        <f t="shared" si="1"/>
+        <v>440 - 470</v>
+      </c>
     </row>
-    <row r="12" spans="1:331" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:335" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>2111</v>
       </c>
@@ -13284,8 +13213,20 @@
       <c r="KL12">
         <v>2044</v>
       </c>
+      <c r="LU12">
+        <f t="shared" si="2"/>
+        <v>4700</v>
+      </c>
+      <c r="LV12">
+        <f t="shared" si="0"/>
+        <v>413</v>
+      </c>
+      <c r="LW12" t="str">
+        <f t="shared" si="1"/>
+        <v>470 - 500</v>
+      </c>
     </row>
-    <row r="13" spans="1:331" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:335" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>1736</v>
       </c>
@@ -14213,8 +14154,20 @@
       <c r="KW13">
         <v>2041</v>
       </c>
+      <c r="LU13">
+        <f t="shared" si="2"/>
+        <v>5000</v>
+      </c>
+      <c r="LV13">
+        <f t="shared" si="0"/>
+        <v>336</v>
+      </c>
+      <c r="LW13" t="str">
+        <f t="shared" si="1"/>
+        <v>500 - 530</v>
+      </c>
     </row>
-    <row r="14" spans="1:331" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:335" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>1804</v>
       </c>
@@ -15169,8 +15122,20 @@
       <c r="LF14">
         <v>2279</v>
       </c>
+      <c r="LU14">
+        <f t="shared" si="2"/>
+        <v>5300</v>
+      </c>
+      <c r="LV14">
+        <f t="shared" si="0"/>
+        <v>164</v>
+      </c>
+      <c r="LW14" t="str">
+        <f t="shared" si="1"/>
+        <v>530 - 560</v>
+      </c>
     </row>
-    <row r="15" spans="1:331" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:335" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>1610</v>
       </c>
@@ -16110,8 +16075,20 @@
       <c r="LA15">
         <v>2309</v>
       </c>
+      <c r="LU15">
+        <f t="shared" si="2"/>
+        <v>5600</v>
+      </c>
+      <c r="LV15">
+        <f t="shared" si="0"/>
+        <v>75</v>
+      </c>
+      <c r="LW15" t="str">
+        <f t="shared" si="1"/>
+        <v>560 - 590</v>
+      </c>
     </row>
-    <row r="16" spans="1:331" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:335" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>1981</v>
       </c>
@@ -16988,8 +16965,20 @@
       <c r="KF16">
         <v>2556</v>
       </c>
+      <c r="LU16">
+        <f t="shared" si="2"/>
+        <v>5900</v>
+      </c>
+      <c r="LV16">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+      <c r="LW16" t="str">
+        <f t="shared" si="1"/>
+        <v>590 - 620</v>
+      </c>
     </row>
-    <row r="17" spans="1:324" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:335" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>1771</v>
       </c>
@@ -17923,8 +17912,20 @@
       <c r="KY17">
         <v>2680</v>
       </c>
+      <c r="LU17">
+        <f t="shared" si="2"/>
+        <v>6200</v>
+      </c>
+      <c r="LV17">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="LW17" t="str">
+        <f t="shared" si="1"/>
+        <v>620 - 650</v>
+      </c>
     </row>
-    <row r="18" spans="1:324" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:335" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>2133</v>
       </c>
@@ -18852,8 +18853,20 @@
       <c r="KW18">
         <v>2218</v>
       </c>
+      <c r="LU18">
+        <f t="shared" si="2"/>
+        <v>6500</v>
+      </c>
+      <c r="LV18">
+        <f t="shared" si="0"/>
+        <v>28</v>
+      </c>
+      <c r="LW18" t="str">
+        <f>"&gt;"&amp;LU18/10</f>
+        <v>&gt;650</v>
+      </c>
     </row>
-    <row r="19" spans="1:324" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:335" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>1835</v>
       </c>
@@ -19695,7 +19708,7 @@
         <v>2547</v>
       </c>
     </row>
-    <row r="20" spans="1:324" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:335" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>1570</v>
       </c>
@@ -20621,7 +20634,7 @@
         <v>3040</v>
       </c>
     </row>
-    <row r="21" spans="1:324" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:335" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>1772</v>
       </c>
@@ -21565,7 +21578,7 @@
         <v>2216</v>
       </c>
     </row>
-    <row r="22" spans="1:324" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:335" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>1877</v>
       </c>
@@ -22464,7 +22477,7 @@
         <v>1924</v>
       </c>
     </row>
-    <row r="23" spans="1:324" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:335" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>2333</v>
       </c>
@@ -23414,7 +23427,7 @@
         <v>2092</v>
       </c>
     </row>
-    <row r="24" spans="1:324" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:335" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>1744</v>
       </c>
@@ -24370,7 +24383,7 @@
         <v>2190</v>
       </c>
     </row>
-    <row r="25" spans="1:324" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:335" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>2330</v>
       </c>
@@ -25335,7 +25348,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="26" spans="1:324" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:335" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>1822</v>
       </c>
@@ -26252,7 +26265,7 @@
         <v>2027</v>
       </c>
     </row>
-    <row r="27" spans="1:324" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:335" x14ac:dyDescent="0.35">
       <c r="A27">
         <v>2491</v>
       </c>
@@ -27190,7 +27203,7 @@
         <v>2347</v>
       </c>
     </row>
-    <row r="28" spans="1:324" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:335" x14ac:dyDescent="0.35">
       <c r="A28">
         <v>2192</v>
       </c>
@@ -28083,7 +28096,7 @@
         <v>2816</v>
       </c>
     </row>
-    <row r="29" spans="1:324" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:335" x14ac:dyDescent="0.35">
       <c r="A29">
         <v>2484</v>
       </c>
@@ -29057,7 +29070,7 @@
         <v>1878</v>
       </c>
     </row>
-    <row r="30" spans="1:324" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:335" x14ac:dyDescent="0.35">
       <c r="A30">
         <v>1585</v>
       </c>

</xml_diff>

<commit_message>
updated presentation and results files
</commit_message>
<xml_diff>
--- a/results1.xlsx
+++ b/results1.xlsx
@@ -14,38 +14,6 @@
   <sheets>
     <sheet name="results1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlchart.v1.0" hidden="1">results1!$A$10:$LS$10</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">results1!$A$11:$LS$11</definedName>
-    <definedName name="_xlchart.v1.10" hidden="1">results1!$A$1:$LS$1</definedName>
-    <definedName name="_xlchart.v1.11" hidden="1">results1!$A$20:$LS$20</definedName>
-    <definedName name="_xlchart.v1.12" hidden="1">results1!$A$21:$LS$21</definedName>
-    <definedName name="_xlchart.v1.13" hidden="1">results1!$A$22:$LS$22</definedName>
-    <definedName name="_xlchart.v1.14" hidden="1">results1!$A$23:$LS$23</definedName>
-    <definedName name="_xlchart.v1.15" hidden="1">results1!$A$24:$LS$24</definedName>
-    <definedName name="_xlchart.v1.16" hidden="1">results1!$A$25:$LS$25</definedName>
-    <definedName name="_xlchart.v1.17" hidden="1">results1!$A$26:$LS$26</definedName>
-    <definedName name="_xlchart.v1.18" hidden="1">results1!$A$27:$LS$27</definedName>
-    <definedName name="_xlchart.v1.19" hidden="1">results1!$A$28:$LS$28</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">results1!$A$12:$LS$12</definedName>
-    <definedName name="_xlchart.v1.20" hidden="1">results1!$A$29:$LS$29</definedName>
-    <definedName name="_xlchart.v1.21" hidden="1">results1!$A$2:$LS$2</definedName>
-    <definedName name="_xlchart.v1.22" hidden="1">results1!$A$30:$LS$30</definedName>
-    <definedName name="_xlchart.v1.23" hidden="1">results1!$A$3:$LS$3</definedName>
-    <definedName name="_xlchart.v1.24" hidden="1">results1!$A$4:$LS$4</definedName>
-    <definedName name="_xlchart.v1.25" hidden="1">results1!$A$5:$LS$5</definedName>
-    <definedName name="_xlchart.v1.26" hidden="1">results1!$A$6:$LS$6</definedName>
-    <definedName name="_xlchart.v1.27" hidden="1">results1!$A$7:$LS$7</definedName>
-    <definedName name="_xlchart.v1.28" hidden="1">results1!$A$8:$LS$8</definedName>
-    <definedName name="_xlchart.v1.29" hidden="1">results1!$A$9:$LS$9</definedName>
-    <definedName name="_xlchart.v1.3" hidden="1">results1!$A$13:$LS$13</definedName>
-    <definedName name="_xlchart.v1.4" hidden="1">results1!$A$14:$LS$14</definedName>
-    <definedName name="_xlchart.v1.5" hidden="1">results1!$A$15:$LS$15</definedName>
-    <definedName name="_xlchart.v1.6" hidden="1">results1!$A$16:$LS$16</definedName>
-    <definedName name="_xlchart.v1.7" hidden="1">results1!$A$17:$LS$17</definedName>
-    <definedName name="_xlchart.v1.8" hidden="1">results1!$A$18:$LS$18</definedName>
-    <definedName name="_xlchart.v1.9" hidden="1">results1!$A$19:$LS$19</definedName>
-  </definedNames>
   <calcPr calcId="171027"/>
 </workbook>
 </file>
@@ -865,7 +833,7 @@
           <a:effectLst/>
         </c:spPr>
         <c:txPr>
-          <a:bodyPr rot="-2700000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:bodyPr rot="-2700000" spcFirstLastPara="1" vertOverflow="ellipsis" wrap="square" anchor="ctr" anchorCtr="1"/>
           <a:lstStyle/>
           <a:p>
             <a:pPr>
@@ -1932,8 +1900,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:LW30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="LF1" workbookViewId="0">
-      <selection activeCell="LN19" sqref="LN19"/>
+    <sheetView tabSelected="1" topLeftCell="LO1" workbookViewId="0">
+      <selection activeCell="LW2" sqref="LW2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>